<commit_message>
fix: comprehensive notebook syntax and import error fixes
- Fixed 500+ notebooks with syntax errors (imports, print statements, string literals)
- Fixed double 'from' import errors in 243 notebooks
- Fixed print statement syntax errors in 215 notebooks
- All required packages installed (sklearn, keras, torch, gym, rdflib, transformers, spacy)
- Current pass rate: 62.2% (508/817), with fixes applied should improve significantly

Fixes address:
- Broken import statements with line breaks
- Unterminated string literals in print statements
- Missing newlines in code
- Double 'from' keywords in imports
- Print statement syntax errors
</commit_message>
<xml_diff>
--- a/unit2-cleaning/examples/sample_data.xlsx
+++ b/unit2-cleaning/examples/sample_data.xlsx
@@ -334,16 +334,16 @@
     <t>Person_100</t>
   </si>
   <si>
+    <t>Sales</t>
+  </si>
+  <si>
+    <t>IT</t>
+  </si>
+  <si>
+    <t>Finance</t>
+  </si>
+  <si>
     <t>HR</t>
-  </si>
-  <si>
-    <t>IT</t>
-  </si>
-  <si>
-    <t>Sales</t>
-  </si>
-  <si>
-    <t>Finance</t>
   </si>
 </sst>
 </file>
@@ -739,10 +739,10 @@
         <v>6</v>
       </c>
       <c r="C2">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D2">
-        <v>92684.39698235976</v>
+        <v>48747.18225563578</v>
       </c>
       <c r="E2" t="s">
         <v>106</v>
@@ -759,13 +759,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D3">
-        <v>56355.33447508394</v>
+        <v>30115.39204226672</v>
       </c>
       <c r="E3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F3" s="2">
         <v>43832</v>
@@ -779,10 +779,10 @@
         <v>8</v>
       </c>
       <c r="C4">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="D4">
-        <v>70844.69346491422</v>
+        <v>41748.34994549691</v>
       </c>
       <c r="E4" t="s">
         <v>107</v>
@@ -799,13 +799,13 @@
         <v>9</v>
       </c>
       <c r="C5">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="D5">
-        <v>47724.98177596941</v>
+        <v>28919.53431584542</v>
       </c>
       <c r="E5" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F5" s="2">
         <v>43834</v>
@@ -819,10 +819,10 @@
         <v>10</v>
       </c>
       <c r="C6">
-        <v>64</v>
+        <v>37</v>
       </c>
       <c r="D6">
-        <v>58737.43495632033</v>
+        <v>47328.46828840613</v>
       </c>
       <c r="E6" t="s">
         <v>106</v>
@@ -839,13 +839,13 @@
         <v>11</v>
       </c>
       <c r="C7">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D7">
-        <v>35961.99175649295</v>
+        <v>27633.67032192531</v>
       </c>
       <c r="E7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F7" s="2">
         <v>43836</v>
@@ -862,7 +862,7 @@
         <v>68</v>
       </c>
       <c r="D8">
-        <v>30949.22422136868</v>
+        <v>38923.80875683604</v>
       </c>
       <c r="E8" t="s">
         <v>108</v>
@@ -879,10 +879,10 @@
         <v>13</v>
       </c>
       <c r="C9">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D9">
-        <v>34484.27762462835</v>
+        <v>66166.54689679258</v>
       </c>
       <c r="E9" t="s">
         <v>109</v>
@@ -899,10 +899,10 @@
         <v>14</v>
       </c>
       <c r="C10">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="D10">
-        <v>48120.87485241259</v>
+        <v>42229.91875356604</v>
       </c>
       <c r="E10" t="s">
         <v>106</v>
@@ -919,13 +919,13 @@
         <v>15</v>
       </c>
       <c r="C11">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="D11">
-        <v>39477.49935563741</v>
+        <v>53676.41526129905</v>
       </c>
       <c r="E11" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F11" s="2">
         <v>43840</v>
@@ -939,13 +939,13 @@
         <v>16</v>
       </c>
       <c r="C12">
-        <v>36</v>
+        <v>65</v>
       </c>
       <c r="D12">
-        <v>54765.68841917362</v>
+        <v>54608.44877630944</v>
       </c>
       <c r="E12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F12" s="2">
         <v>43841</v>
@@ -959,13 +959,13 @@
         <v>17</v>
       </c>
       <c r="C13">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="D13">
-        <v>65050.41549822858</v>
+        <v>44604.76962374042</v>
       </c>
       <c r="E13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F13" s="2">
         <v>43842</v>
@@ -979,13 +979,13 @@
         <v>18</v>
       </c>
       <c r="C14">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D14">
-        <v>36002.48895065899</v>
+        <v>62124.99708616879</v>
       </c>
       <c r="E14" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="F14" s="2">
         <v>43843</v>
@@ -999,10 +999,10 @@
         <v>19</v>
       </c>
       <c r="C15">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="D15">
-        <v>51612.59561630987</v>
+        <v>62627.20076670023</v>
       </c>
       <c r="E15" t="s">
         <v>108</v>
@@ -1019,13 +1019,13 @@
         <v>20</v>
       </c>
       <c r="C16">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D16">
-        <v>44558.34481603771</v>
+        <v>59138.32754534869</v>
       </c>
       <c r="E16" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F16" s="2">
         <v>43845</v>
@@ -1039,13 +1039,13 @@
         <v>21</v>
       </c>
       <c r="C17">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D17">
-        <v>63975.13552902873</v>
+        <v>33641.82103386788</v>
       </c>
       <c r="E17" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="F17" s="2">
         <v>43846</v>
@@ -1059,13 +1059,13 @@
         <v>22</v>
       </c>
       <c r="C18">
-        <v>59</v>
+        <v>28</v>
       </c>
       <c r="D18">
-        <v>20720.00792692635</v>
+        <v>49043.63139532429</v>
       </c>
       <c r="E18" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F18" s="2">
         <v>43847</v>
@@ -1079,13 +1079,13 @@
         <v>23</v>
       </c>
       <c r="C19">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="D19">
-        <v>59201.07630295688</v>
+        <v>56847.59821639571</v>
       </c>
       <c r="E19" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F19" s="2">
         <v>43848</v>
@@ -1099,13 +1099,13 @@
         <v>24</v>
       </c>
       <c r="C20">
-        <v>31</v>
+        <v>55</v>
       </c>
       <c r="D20">
-        <v>102512.8185659996</v>
+        <v>42274.05384377464</v>
       </c>
       <c r="E20" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F20" s="2">
         <v>43849</v>
@@ -1119,10 +1119,10 @@
         <v>25</v>
       </c>
       <c r="C21">
-        <v>64</v>
+        <v>24</v>
       </c>
       <c r="D21">
-        <v>41179.84920320375</v>
+        <v>68393.99577512604</v>
       </c>
       <c r="E21" t="s">
         <v>108</v>
@@ -1139,10 +1139,10 @@
         <v>26</v>
       </c>
       <c r="C22">
-        <v>38</v>
+        <v>60</v>
       </c>
       <c r="D22">
-        <v>70052.36526063706</v>
+        <v>46966.98717729333</v>
       </c>
       <c r="E22" t="s">
         <v>106</v>
@@ -1159,13 +1159,13 @@
         <v>27</v>
       </c>
       <c r="C23">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D23">
-        <v>61691.98876082872</v>
+        <v>45037.35445987143</v>
       </c>
       <c r="E23" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F23" s="2">
         <v>43852</v>
@@ -1179,13 +1179,13 @@
         <v>28</v>
       </c>
       <c r="C24">
-        <v>72</v>
+        <v>47</v>
       </c>
       <c r="D24">
-        <v>53690.72502402482</v>
+        <v>25125.24721837497</v>
       </c>
       <c r="E24" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F24" s="2">
         <v>43853</v>
@@ -1199,13 +1199,13 @@
         <v>29</v>
       </c>
       <c r="C25">
-        <v>21</v>
+        <v>79</v>
       </c>
       <c r="D25">
-        <v>37237.29626160867</v>
+        <v>29474.0067394532</v>
       </c>
       <c r="E25" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F25" s="2">
         <v>43854</v>
@@ -1219,13 +1219,13 @@
         <v>30</v>
       </c>
       <c r="C26">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="D26">
-        <v>31314.50446296222</v>
+        <v>58712.33365640082</v>
       </c>
       <c r="E26" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F26" s="2">
         <v>43855</v>
@@ -1239,10 +1239,10 @@
         <v>31</v>
       </c>
       <c r="C27">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="D27">
-        <v>36329.62826776807</v>
+        <v>70269.52866785933</v>
       </c>
       <c r="E27" t="s">
         <v>109</v>
@@ -1259,13 +1259,13 @@
         <v>32</v>
       </c>
       <c r="C28">
-        <v>59</v>
+        <v>36</v>
       </c>
       <c r="D28">
-        <v>35416.79922626989</v>
+        <v>56227.08707745132</v>
       </c>
       <c r="E28" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F28" s="2">
         <v>43857</v>
@@ -1279,13 +1279,13 @@
         <v>33</v>
       </c>
       <c r="C29">
-        <v>65</v>
+        <v>23</v>
       </c>
       <c r="D29">
-        <v>44168.04856387572</v>
+        <v>63885.03663094122</v>
       </c>
       <c r="E29" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F29" s="2">
         <v>43858</v>
@@ -1299,13 +1299,13 @@
         <v>34</v>
       </c>
       <c r="C30">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="D30">
-        <v>60296.63736910241</v>
+        <v>52077.74816613758</v>
       </c>
       <c r="E30" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F30" s="2">
         <v>43859</v>
@@ -1319,13 +1319,13 @@
         <v>35</v>
       </c>
       <c r="C31">
-        <v>61</v>
+        <v>33</v>
       </c>
       <c r="D31">
-        <v>66752.34346992857</v>
+        <v>42505.01488833394</v>
       </c>
       <c r="E31" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F31" s="2">
         <v>43860</v>
@@ -1339,10 +1339,10 @@
         <v>36</v>
       </c>
       <c r="C32">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="D32">
-        <v>77091.59888507298</v>
+        <v>58338.250549846</v>
       </c>
       <c r="E32" t="s">
         <v>107</v>
@@ -1359,13 +1359,13 @@
         <v>37</v>
       </c>
       <c r="C33">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D33">
-        <v>67464.83526382498</v>
+        <v>58961.62394646474</v>
       </c>
       <c r="E33" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="F33" s="2">
         <v>43862</v>
@@ -1379,13 +1379,13 @@
         <v>38</v>
       </c>
       <c r="C34">
-        <v>40</v>
+        <v>78</v>
       </c>
       <c r="D34">
-        <v>35217.88733441991</v>
+        <v>50474.76445185542</v>
       </c>
       <c r="E34" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F34" s="2">
         <v>43863</v>
@@ -1399,13 +1399,13 @@
         <v>39</v>
       </c>
       <c r="C35">
-        <v>60</v>
+        <v>39</v>
       </c>
       <c r="D35">
-        <v>64466.7385833465</v>
+        <v>45200.74095117793</v>
       </c>
       <c r="E35" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F35" s="2">
         <v>43864</v>
@@ -1419,13 +1419,13 @@
         <v>40</v>
       </c>
       <c r="C36">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="D36">
-        <v>60179.73537126673</v>
+        <v>76871.29837205488</v>
       </c>
       <c r="E36" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F36" s="2">
         <v>43865</v>
@@ -1439,10 +1439,10 @@
         <v>41</v>
       </c>
       <c r="C37">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="D37">
-        <v>63399.71327550809</v>
+        <v>53810.28041161156</v>
       </c>
       <c r="E37" t="s">
         <v>106</v>
@@ -1459,13 +1459,13 @@
         <v>42</v>
       </c>
       <c r="C38">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D38">
-        <v>46432.83482478911</v>
+        <v>43970.71778374718</v>
       </c>
       <c r="E38" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F38" s="2">
         <v>43867</v>
@@ -1479,13 +1479,13 @@
         <v>43</v>
       </c>
       <c r="C39">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="D39">
-        <v>48397.50658657567</v>
+        <v>50066.52584702597</v>
       </c>
       <c r="E39" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F39" s="2">
         <v>43868</v>
@@ -1499,10 +1499,10 @@
         <v>44</v>
       </c>
       <c r="C40">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D40">
-        <v>71624.72405771201</v>
+        <v>50628.88656703735</v>
       </c>
       <c r="E40" t="s">
         <v>109</v>
@@ -1519,13 +1519,13 @@
         <v>45</v>
       </c>
       <c r="C41">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="D41">
-        <v>25394.96529441418</v>
+        <v>35728.47694440125</v>
       </c>
       <c r="E41" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="F41" s="2">
         <v>43870</v>
@@ -1539,10 +1539,10 @@
         <v>46</v>
       </c>
       <c r="C42">
-        <v>54</v>
+        <v>33</v>
       </c>
       <c r="D42">
-        <v>47344.80995341913</v>
+        <v>46194.82902647479</v>
       </c>
       <c r="E42" t="s">
         <v>109</v>
@@ -1559,13 +1559,13 @@
         <v>47</v>
       </c>
       <c r="C43">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D43">
-        <v>53777.71186097637</v>
+        <v>85882.90804363557</v>
       </c>
       <c r="E43" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F43" s="2">
         <v>43872</v>
@@ -1579,13 +1579,13 @@
         <v>48</v>
       </c>
       <c r="C44">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="D44">
-        <v>43744.31875895497</v>
+        <v>81673.83793967988</v>
       </c>
       <c r="E44" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F44" s="2">
         <v>43873</v>
@@ -1599,13 +1599,13 @@
         <v>49</v>
       </c>
       <c r="C45">
-        <v>70</v>
+        <v>42</v>
       </c>
       <c r="D45">
-        <v>51898.76889126191</v>
+        <v>51089.47488489129</v>
       </c>
       <c r="E45" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F45" s="2">
         <v>43874</v>
@@ -1619,13 +1619,13 @@
         <v>50</v>
       </c>
       <c r="C46">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="D46">
-        <v>49926.54743339906</v>
+        <v>17160.39650100514</v>
       </c>
       <c r="E46" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F46" s="2">
         <v>43875</v>
@@ -1639,13 +1639,13 @@
         <v>51</v>
       </c>
       <c r="C47">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="D47">
-        <v>34284.86413479479</v>
+        <v>61563.04219691779</v>
       </c>
       <c r="E47" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F47" s="2">
         <v>43876</v>
@@ -1659,10 +1659,10 @@
         <v>52</v>
       </c>
       <c r="C48">
-        <v>71</v>
+        <v>44</v>
       </c>
       <c r="D48">
-        <v>28474.35365323645</v>
+        <v>53360.38571940515</v>
       </c>
       <c r="E48" t="s">
         <v>106</v>
@@ -1679,10 +1679,10 @@
         <v>53</v>
       </c>
       <c r="C49">
-        <v>48</v>
+        <v>72</v>
       </c>
       <c r="D49">
-        <v>57731.82870877686</v>
+        <v>51008.23630018337</v>
       </c>
       <c r="E49" t="s">
         <v>109</v>
@@ -1699,13 +1699,13 @@
         <v>54</v>
       </c>
       <c r="C50">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="D50">
-        <v>56813.68964183124</v>
+        <v>47948.04113218602</v>
       </c>
       <c r="E50" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F50" s="2">
         <v>43879</v>
@@ -1719,13 +1719,13 @@
         <v>55</v>
       </c>
       <c r="C51">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D51">
-        <v>48733.08115833197</v>
+        <v>67014.63247384084</v>
       </c>
       <c r="E51" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="F51" s="2">
         <v>43880</v>
@@ -1739,13 +1739,13 @@
         <v>56</v>
       </c>
       <c r="C52">
-        <v>27</v>
+        <v>77</v>
       </c>
       <c r="D52">
-        <v>62010.0687402745</v>
+        <v>70709.92284020971</v>
       </c>
       <c r="E52" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="F52" s="2">
         <v>43881</v>
@@ -1759,13 +1759,13 @@
         <v>57</v>
       </c>
       <c r="C53">
-        <v>71</v>
+        <v>40</v>
       </c>
       <c r="D53">
-        <v>41706.58391683771</v>
+        <v>44823.78157863708</v>
       </c>
       <c r="E53" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F53" s="2">
         <v>43882</v>
@@ -1779,10 +1779,10 @@
         <v>58</v>
       </c>
       <c r="C54">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="D54">
-        <v>72064.84878902925</v>
+        <v>44311.38369641478</v>
       </c>
       <c r="E54" t="s">
         <v>108</v>
@@ -1799,13 +1799,13 @@
         <v>59</v>
       </c>
       <c r="C55">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D55">
-        <v>69009.69688601894</v>
+        <v>56194.24908299612</v>
       </c>
       <c r="E55" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="F55" s="2">
         <v>43884</v>
@@ -1819,10 +1819,10 @@
         <v>60</v>
       </c>
       <c r="C56">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="D56">
-        <v>71135.09672451419</v>
+        <v>62691.97149345225</v>
       </c>
       <c r="E56" t="s">
         <v>109</v>
@@ -1839,13 +1839,13 @@
         <v>61</v>
       </c>
       <c r="C57">
-        <v>57</v>
+        <v>74</v>
       </c>
       <c r="D57">
-        <v>31245.54300822557</v>
+        <v>43975.33382417331</v>
       </c>
       <c r="E57" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F57" s="2">
         <v>43886</v>
@@ -1859,13 +1859,13 @@
         <v>62</v>
       </c>
       <c r="C58">
-        <v>72</v>
+        <v>29</v>
       </c>
       <c r="D58">
-        <v>58962.48200924</v>
+        <v>45875.84727537336</v>
       </c>
       <c r="E58" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F58" s="2">
         <v>43887</v>
@@ -1879,13 +1879,13 @@
         <v>63</v>
       </c>
       <c r="C59">
-        <v>19</v>
+        <v>70</v>
       </c>
       <c r="D59">
-        <v>56953.56644506898</v>
+        <v>52935.84542437725</v>
       </c>
       <c r="E59" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="F59" s="2">
         <v>43888</v>
@@ -1902,10 +1902,10 @@
         <v>25</v>
       </c>
       <c r="D60">
-        <v>42664.98600496077</v>
+        <v>45230.50155226173</v>
       </c>
       <c r="E60" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F60" s="2">
         <v>43889</v>
@@ -1919,10 +1919,10 @@
         <v>65</v>
       </c>
       <c r="C61">
-        <v>18</v>
+        <v>77</v>
       </c>
       <c r="D61">
-        <v>66146.92624570361</v>
+        <v>46375.19437984942</v>
       </c>
       <c r="E61" t="s">
         <v>109</v>
@@ -1939,13 +1939,13 @@
         <v>66</v>
       </c>
       <c r="C62">
-        <v>40</v>
+        <v>69</v>
       </c>
       <c r="D62">
-        <v>55747.29010388995</v>
+        <v>81805.78806199362</v>
       </c>
       <c r="E62" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F62" s="2">
         <v>43891</v>
@@ -1959,10 +1959,10 @@
         <v>67</v>
       </c>
       <c r="C63">
-        <v>70</v>
+        <v>19</v>
       </c>
       <c r="D63">
-        <v>30712.5071566054</v>
+        <v>51958.882278378</v>
       </c>
       <c r="E63" t="s">
         <v>107</v>
@@ -1979,13 +1979,13 @@
         <v>68</v>
       </c>
       <c r="C64">
-        <v>23</v>
+        <v>64</v>
       </c>
       <c r="D64">
-        <v>45676.28186129322</v>
+        <v>60772.7495886137</v>
       </c>
       <c r="E64" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="F64" s="2">
         <v>43893</v>
@@ -1999,13 +1999,13 @@
         <v>69</v>
       </c>
       <c r="C65">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="D65">
-        <v>65138.09130879585</v>
+        <v>72523.1779111428</v>
       </c>
       <c r="E65" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F65" s="2">
         <v>43894</v>
@@ -2019,10 +2019,10 @@
         <v>70</v>
       </c>
       <c r="C66">
-        <v>38</v>
+        <v>60</v>
       </c>
       <c r="D66">
-        <v>55751.58774503604</v>
+        <v>54409.09634286517</v>
       </c>
       <c r="E66" t="s">
         <v>109</v>
@@ -2039,10 +2039,10 @@
         <v>71</v>
       </c>
       <c r="C67">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D67">
-        <v>68261.46605012364</v>
+        <v>71138.43177575147</v>
       </c>
       <c r="E67" t="s">
         <v>106</v>
@@ -2059,10 +2059,10 @@
         <v>72</v>
       </c>
       <c r="C68">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D68">
-        <v>30180.08126333683</v>
+        <v>58002.39667828627</v>
       </c>
       <c r="E68" t="s">
         <v>106</v>
@@ -2079,13 +2079,13 @@
         <v>73</v>
       </c>
       <c r="C69">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="D69">
-        <v>27406.51801353252</v>
+        <v>42229.13039219988</v>
       </c>
       <c r="E69" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="F69" s="2">
         <v>43898</v>
@@ -2099,13 +2099,13 @@
         <v>74</v>
       </c>
       <c r="C70">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="D70">
-        <v>56283.9046534248</v>
+        <v>33100.17028626416</v>
       </c>
       <c r="E70" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F70" s="2">
         <v>43899</v>
@@ -2119,13 +2119,13 @@
         <v>75</v>
       </c>
       <c r="C71">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D71">
-        <v>32756.34989883802</v>
+        <v>35927.28971255108</v>
       </c>
       <c r="E71" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F71" s="2">
         <v>43900</v>
@@ -2139,13 +2139,13 @@
         <v>76</v>
       </c>
       <c r="C72">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D72">
-        <v>54995.06453482284</v>
+        <v>79779.14480813245</v>
       </c>
       <c r="E72" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="F72" s="2">
         <v>43901</v>
@@ -2159,10 +2159,10 @@
         <v>77</v>
       </c>
       <c r="C73">
-        <v>18</v>
+        <v>56</v>
       </c>
       <c r="D73">
-        <v>67214.99592701741</v>
+        <v>62753.8276106726</v>
       </c>
       <c r="E73" t="s">
         <v>109</v>
@@ -2179,10 +2179,10 @@
         <v>78</v>
       </c>
       <c r="C74">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="D74">
-        <v>17039.73126962649</v>
+        <v>44413.54666275848</v>
       </c>
       <c r="E74" t="s">
         <v>109</v>
@@ -2199,13 +2199,13 @@
         <v>79</v>
       </c>
       <c r="C75">
-        <v>44</v>
+        <v>69</v>
       </c>
       <c r="D75">
-        <v>45406.31903680969</v>
+        <v>60504.17068824657</v>
       </c>
       <c r="E75" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F75" s="2">
         <v>43904</v>
@@ -2219,13 +2219,13 @@
         <v>80</v>
       </c>
       <c r="C76">
-        <v>75</v>
+        <v>49</v>
       </c>
       <c r="D76">
-        <v>67278.27403564543</v>
+        <v>69815.43867979474</v>
       </c>
       <c r="E76" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="F76" s="2">
         <v>43905</v>
@@ -2239,13 +2239,13 @@
         <v>81</v>
       </c>
       <c r="C77">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D77">
-        <v>49135.90717368644</v>
+        <v>49570.44601291049</v>
       </c>
       <c r="E77" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="F77" s="2">
         <v>43906</v>
@@ -2259,13 +2259,13 @@
         <v>82</v>
       </c>
       <c r="C78">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D78">
-        <v>20657.98323521588</v>
+        <v>62552.59644420939</v>
       </c>
       <c r="E78" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="F78" s="2">
         <v>43907</v>
@@ -2279,13 +2279,13 @@
         <v>83</v>
       </c>
       <c r="C79">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="D79">
-        <v>31260.12193996227</v>
+        <v>60999.36650136659</v>
       </c>
       <c r="E79" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F79" s="2">
         <v>43908</v>
@@ -2299,10 +2299,10 @@
         <v>84</v>
       </c>
       <c r="C80">
-        <v>74</v>
+        <v>50</v>
       </c>
       <c r="D80">
-        <v>75087.96083644922</v>
+        <v>42116.29517962358</v>
       </c>
       <c r="E80" t="s">
         <v>109</v>
@@ -2319,10 +2319,10 @@
         <v>85</v>
       </c>
       <c r="C81">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D81">
-        <v>57560.87296775137</v>
+        <v>47480.33511445128</v>
       </c>
       <c r="E81" t="s">
         <v>109</v>
@@ -2339,13 +2339,13 @@
         <v>86</v>
       </c>
       <c r="C82">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="D82">
-        <v>38210.68464936284</v>
+        <v>67210.72666778362</v>
       </c>
       <c r="E82" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="F82" s="2">
         <v>43911</v>
@@ -2362,10 +2362,10 @@
         <v>70</v>
       </c>
       <c r="D83">
-        <v>53571.10234168046</v>
+        <v>42132.27539997448</v>
       </c>
       <c r="E83" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F83" s="2">
         <v>43912</v>
@@ -2379,13 +2379,13 @@
         <v>88</v>
       </c>
       <c r="C84">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="D84">
-        <v>81482.81131204928</v>
+        <v>45738.73883513115</v>
       </c>
       <c r="E84" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="F84" s="2">
         <v>43913</v>
@@ -2399,10 +2399,10 @@
         <v>89</v>
       </c>
       <c r="C85">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="D85">
-        <v>39267.64990419869</v>
+        <v>66469.08386290674</v>
       </c>
       <c r="E85" t="s">
         <v>108</v>
@@ -2419,13 +2419,13 @@
         <v>90</v>
       </c>
       <c r="C86">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="D86">
-        <v>28944.28700429525</v>
+        <v>40558.44006106135</v>
       </c>
       <c r="E86" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F86" s="2">
         <v>43915</v>
@@ -2439,13 +2439,13 @@
         <v>91</v>
       </c>
       <c r="C87">
-        <v>76</v>
+        <v>24</v>
       </c>
       <c r="D87">
-        <v>56568.35607789297</v>
+        <v>34384.61200073149</v>
       </c>
       <c r="E87" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F87" s="2">
         <v>43916</v>
@@ -2459,10 +2459,10 @@
         <v>92</v>
       </c>
       <c r="C88">
-        <v>73</v>
+        <v>54</v>
       </c>
       <c r="D88">
-        <v>45044.45073943168</v>
+        <v>63132.1742196581</v>
       </c>
       <c r="E88" t="s">
         <v>107</v>
@@ -2479,13 +2479,13 @@
         <v>93</v>
       </c>
       <c r="C89">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D89">
-        <v>38602.88926932471</v>
+        <v>44166.57388944553</v>
       </c>
       <c r="E89" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F89" s="2">
         <v>43918</v>
@@ -2499,10 +2499,10 @@
         <v>94</v>
       </c>
       <c r="C90">
-        <v>72</v>
+        <v>27</v>
       </c>
       <c r="D90">
-        <v>73554.99173124704</v>
+        <v>49508.16176961461</v>
       </c>
       <c r="E90" t="s">
         <v>106</v>
@@ -2519,13 +2519,13 @@
         <v>95</v>
       </c>
       <c r="C91">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D91">
-        <v>43905.98624356584</v>
+        <v>70411.33857364788</v>
       </c>
       <c r="E91" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F91" s="2">
         <v>43920</v>
@@ -2539,10 +2539,10 @@
         <v>96</v>
       </c>
       <c r="C92">
-        <v>77</v>
+        <v>39</v>
       </c>
       <c r="D92">
-        <v>27623.77190437306</v>
+        <v>45340.90359442343</v>
       </c>
       <c r="E92" t="s">
         <v>106</v>
@@ -2559,13 +2559,13 @@
         <v>97</v>
       </c>
       <c r="C93">
-        <v>19</v>
+        <v>58</v>
       </c>
       <c r="D93">
-        <v>39546.51764575763</v>
+        <v>61177.84262268715</v>
       </c>
       <c r="E93" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F93" s="2">
         <v>43922</v>
@@ -2579,13 +2579,13 @@
         <v>98</v>
       </c>
       <c r="C94">
-        <v>22</v>
+        <v>47</v>
       </c>
       <c r="D94">
-        <v>61948.41031895989</v>
+        <v>34253.9722916211</v>
       </c>
       <c r="E94" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F94" s="2">
         <v>43923</v>
@@ -2599,13 +2599,13 @@
         <v>99</v>
       </c>
       <c r="C95">
-        <v>67</v>
+        <v>37</v>
       </c>
       <c r="D95">
-        <v>50155.12179346532</v>
+        <v>76485.02388135628</v>
       </c>
       <c r="E95" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="F95" s="2">
         <v>43924</v>
@@ -2619,10 +2619,10 @@
         <v>100</v>
       </c>
       <c r="C96">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D96">
-        <v>32892.39511586259</v>
+        <v>57601.53122227205</v>
       </c>
       <c r="E96" t="s">
         <v>108</v>
@@ -2639,10 +2639,10 @@
         <v>101</v>
       </c>
       <c r="C97">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D97">
-        <v>69780.96042043115</v>
+        <v>45945.4847975202</v>
       </c>
       <c r="E97" t="s">
         <v>108</v>
@@ -2659,13 +2659,13 @@
         <v>102</v>
       </c>
       <c r="C98">
-        <v>20</v>
+        <v>56</v>
       </c>
       <c r="D98">
-        <v>77448.91331598033</v>
+        <v>70612.09564442124</v>
       </c>
       <c r="E98" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F98" s="2">
         <v>43927</v>
@@ -2679,10 +2679,10 @@
         <v>103</v>
       </c>
       <c r="C99">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="D99">
-        <v>39721.75797884333</v>
+        <v>59292.41802552177</v>
       </c>
       <c r="E99" t="s">
         <v>109</v>
@@ -2699,13 +2699,13 @@
         <v>104</v>
       </c>
       <c r="C100">
-        <v>65</v>
+        <v>78</v>
       </c>
       <c r="D100">
-        <v>42448.19423734699</v>
+        <v>51979.50292369697</v>
       </c>
       <c r="E100" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F100" s="2">
         <v>43929</v>
@@ -2719,13 +2719,13 @@
         <v>105</v>
       </c>
       <c r="C101">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="D101">
-        <v>57560.27009022118</v>
+        <v>42914.25124921309</v>
       </c>
       <c r="E101" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="F101" s="2">
         <v>43930</v>

</xml_diff>

<commit_message>
fix: scientific notation fixes - 77.2% passing
- Fixed broken scientific notation patterns (h=1\ne-6 -> h=1e-6)
- Fixed docstring/def merging patterns
- Fixed import/def merging patterns
- 631/817 passing (77.2%)
- +134 notebooks fixed from start
</commit_message>
<xml_diff>
--- a/unit2-cleaning/examples/sample_data.xlsx
+++ b/unit2-cleaning/examples/sample_data.xlsx
@@ -337,13 +337,13 @@
     <t>HR</t>
   </si>
   <si>
+    <t>IT</t>
+  </si>
+  <si>
+    <t>Sales</t>
+  </si>
+  <si>
     <t>Finance</t>
-  </si>
-  <si>
-    <t>Sales</t>
-  </si>
-  <si>
-    <t>IT</t>
   </si>
 </sst>
 </file>
@@ -739,10 +739,10 @@
         <v>6</v>
       </c>
       <c r="C2">
-        <v>79</v>
+        <v>22</v>
       </c>
       <c r="D2">
-        <v>71413.25750831426</v>
+        <v>44960.27464322234</v>
       </c>
       <c r="E2" t="s">
         <v>106</v>
@@ -759,10 +759,10 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="D3">
-        <v>67798.26638645779</v>
+        <v>57943.52576821176</v>
       </c>
       <c r="E3" t="s">
         <v>107</v>
@@ -779,13 +779,13 @@
         <v>8</v>
       </c>
       <c r="C4">
-        <v>63</v>
+        <v>36</v>
       </c>
       <c r="D4">
-        <v>43146.63699099272</v>
+        <v>31319.79348588433</v>
       </c>
       <c r="E4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F4" s="2">
         <v>43833</v>
@@ -799,13 +799,13 @@
         <v>9</v>
       </c>
       <c r="C5">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="D5">
-        <v>46156.07389635999</v>
+        <v>40179.6619347845</v>
       </c>
       <c r="E5" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F5" s="2">
         <v>43834</v>
@@ -819,10 +819,10 @@
         <v>10</v>
       </c>
       <c r="C6">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="D6">
-        <v>35391.75272279474</v>
+        <v>59650.12426497611</v>
       </c>
       <c r="E6" t="s">
         <v>107</v>
@@ -839,10 +839,10 @@
         <v>11</v>
       </c>
       <c r="C7">
-        <v>56</v>
+        <v>76</v>
       </c>
       <c r="D7">
-        <v>46243.04769028643</v>
+        <v>51052.02502526587</v>
       </c>
       <c r="E7" t="s">
         <v>108</v>
@@ -859,13 +859,13 @@
         <v>12</v>
       </c>
       <c r="C8">
-        <v>79</v>
+        <v>25</v>
       </c>
       <c r="D8">
-        <v>73455.17145579855</v>
+        <v>77093.73624377328</v>
       </c>
       <c r="E8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F8" s="2">
         <v>43837</v>
@@ -879,13 +879,13 @@
         <v>13</v>
       </c>
       <c r="C9">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="D9">
-        <v>29911.32551704424</v>
+        <v>52393.1381577621</v>
       </c>
       <c r="E9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F9" s="2">
         <v>43838</v>
@@ -899,10 +899,10 @@
         <v>14</v>
       </c>
       <c r="C10">
-        <v>21</v>
+        <v>53</v>
       </c>
       <c r="D10">
-        <v>61434.76145507795</v>
+        <v>31611.41661894799</v>
       </c>
       <c r="E10" t="s">
         <v>107</v>
@@ -919,10 +919,10 @@
         <v>15</v>
       </c>
       <c r="C11">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D11">
-        <v>39258.25243781997</v>
+        <v>51004.59882068611</v>
       </c>
       <c r="E11" t="s">
         <v>107</v>
@@ -939,13 +939,13 @@
         <v>16</v>
       </c>
       <c r="C12">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="D12">
-        <v>72228.07441527712</v>
+        <v>46043.63791274435</v>
       </c>
       <c r="E12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F12" s="2">
         <v>43841</v>
@@ -959,13 +959,13 @@
         <v>17</v>
       </c>
       <c r="C13">
-        <v>53</v>
+        <v>18</v>
       </c>
       <c r="D13">
-        <v>38597.54673506894</v>
+        <v>50793.72186306445</v>
       </c>
       <c r="E13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F13" s="2">
         <v>43842</v>
@@ -979,13 +979,13 @@
         <v>18</v>
       </c>
       <c r="C14">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="D14">
-        <v>37218.52314511579</v>
+        <v>73145.36265166868</v>
       </c>
       <c r="E14" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F14" s="2">
         <v>43843</v>
@@ -999,10 +999,10 @@
         <v>19</v>
       </c>
       <c r="C15">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="D15">
-        <v>30138.07637690203</v>
+        <v>46998.02609127467</v>
       </c>
       <c r="E15" t="s">
         <v>108</v>
@@ -1019,13 +1019,13 @@
         <v>20</v>
       </c>
       <c r="C16">
-        <v>72</v>
+        <v>20</v>
       </c>
       <c r="D16">
-        <v>49229.55445186605</v>
+        <v>38994.39797376977</v>
       </c>
       <c r="E16" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F16" s="2">
         <v>43845</v>
@@ -1039,13 +1039,13 @@
         <v>21</v>
       </c>
       <c r="C17">
-        <v>23</v>
+        <v>63</v>
       </c>
       <c r="D17">
-        <v>28988.94010972304</v>
+        <v>43287.7795929508</v>
       </c>
       <c r="E17" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="F17" s="2">
         <v>43846</v>
@@ -1059,13 +1059,13 @@
         <v>22</v>
       </c>
       <c r="C18">
-        <v>36</v>
+        <v>58</v>
       </c>
       <c r="D18">
-        <v>42755.0445777408</v>
+        <v>69026.95026018156</v>
       </c>
       <c r="E18" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="F18" s="2">
         <v>43847</v>
@@ -1079,13 +1079,13 @@
         <v>23</v>
       </c>
       <c r="C19">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="D19">
-        <v>19000.67807757658</v>
+        <v>48152.40511422901</v>
       </c>
       <c r="E19" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F19" s="2">
         <v>43848</v>
@@ -1099,13 +1099,13 @@
         <v>24</v>
       </c>
       <c r="C20">
-        <v>34</v>
+        <v>68</v>
       </c>
       <c r="D20">
-        <v>83821.84999331116</v>
+        <v>34635.40887966212</v>
       </c>
       <c r="E20" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F20" s="2">
         <v>43849</v>
@@ -1119,13 +1119,13 @@
         <v>25</v>
       </c>
       <c r="C21">
-        <v>22</v>
+        <v>68</v>
       </c>
       <c r="D21">
-        <v>36681.39451141895</v>
+        <v>65576.28862785012</v>
       </c>
       <c r="E21" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F21" s="2">
         <v>43850</v>
@@ -1139,13 +1139,13 @@
         <v>26</v>
       </c>
       <c r="C22">
-        <v>40</v>
+        <v>73</v>
       </c>
       <c r="D22">
-        <v>34839.62088522573</v>
+        <v>36338.25300772311</v>
       </c>
       <c r="E22" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F22" s="2">
         <v>43851</v>
@@ -1159,13 +1159,13 @@
         <v>27</v>
       </c>
       <c r="C23">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D23">
-        <v>49504.9900803975</v>
+        <v>60808.22430682303</v>
       </c>
       <c r="E23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F23" s="2">
         <v>43852</v>
@@ -1179,13 +1179,13 @@
         <v>28</v>
       </c>
       <c r="C24">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D24">
-        <v>53393.10461587259</v>
+        <v>30968.96942639022</v>
       </c>
       <c r="E24" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F24" s="2">
         <v>43853</v>
@@ -1199,10 +1199,10 @@
         <v>29</v>
       </c>
       <c r="C25">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D25">
-        <v>35884.15738972933</v>
+        <v>45892.16244925607</v>
       </c>
       <c r="E25" t="s">
         <v>106</v>
@@ -1219,13 +1219,13 @@
         <v>30</v>
       </c>
       <c r="C26">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="D26">
-        <v>61507.95246189561</v>
+        <v>56536.2695358794</v>
       </c>
       <c r="E26" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F26" s="2">
         <v>43855</v>
@@ -1239,13 +1239,13 @@
         <v>31</v>
       </c>
       <c r="C27">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="D27">
-        <v>85633.12579569485</v>
+        <v>26565.89129939054</v>
       </c>
       <c r="E27" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F27" s="2">
         <v>43856</v>
@@ -1259,13 +1259,13 @@
         <v>32</v>
       </c>
       <c r="C28">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="D28">
-        <v>52881.45670126644</v>
+        <v>53314.09707453496</v>
       </c>
       <c r="E28" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F28" s="2">
         <v>43857</v>
@@ -1279,10 +1279,10 @@
         <v>33</v>
       </c>
       <c r="C29">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="D29">
-        <v>28616.00817532434</v>
+        <v>44298.21756685802</v>
       </c>
       <c r="E29" t="s">
         <v>109</v>
@@ -1299,13 +1299,13 @@
         <v>34</v>
       </c>
       <c r="C30">
-        <v>28</v>
+        <v>77</v>
       </c>
       <c r="D30">
-        <v>65933.8905149682</v>
+        <v>44783.96314160818</v>
       </c>
       <c r="E30" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F30" s="2">
         <v>43859</v>
@@ -1319,13 +1319,13 @@
         <v>35</v>
       </c>
       <c r="C31">
-        <v>47</v>
+        <v>79</v>
       </c>
       <c r="D31">
-        <v>88893.27576899443</v>
+        <v>70109.26213877019</v>
       </c>
       <c r="E31" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F31" s="2">
         <v>43860</v>
@@ -1339,13 +1339,13 @@
         <v>36</v>
       </c>
       <c r="C32">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="D32">
-        <v>52440.1580267398</v>
+        <v>43166.0179341811</v>
       </c>
       <c r="E32" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F32" s="2">
         <v>43861</v>
@@ -1359,10 +1359,10 @@
         <v>37</v>
       </c>
       <c r="C33">
-        <v>74</v>
+        <v>52</v>
       </c>
       <c r="D33">
-        <v>66478.87971352902</v>
+        <v>60926.40833863431</v>
       </c>
       <c r="E33" t="s">
         <v>106</v>
@@ -1379,13 +1379,13 @@
         <v>38</v>
       </c>
       <c r="C34">
-        <v>28</v>
+        <v>66</v>
       </c>
       <c r="D34">
-        <v>74483.46429328357</v>
+        <v>48910.55266364686</v>
       </c>
       <c r="E34" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="F34" s="2">
         <v>43863</v>
@@ -1399,13 +1399,13 @@
         <v>39</v>
       </c>
       <c r="C35">
-        <v>39</v>
+        <v>77</v>
       </c>
       <c r="D35">
-        <v>51565.96098312464</v>
+        <v>71647.39885590435</v>
       </c>
       <c r="E35" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="F35" s="2">
         <v>43864</v>
@@ -1419,10 +1419,10 @@
         <v>40</v>
       </c>
       <c r="C36">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="D36">
-        <v>60140.64671038975</v>
+        <v>50169.12010992338</v>
       </c>
       <c r="E36" t="s">
         <v>106</v>
@@ -1439,10 +1439,10 @@
         <v>41</v>
       </c>
       <c r="C37">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="D37">
-        <v>62807.15018612202</v>
+        <v>37201.54164423887</v>
       </c>
       <c r="E37" t="s">
         <v>107</v>
@@ -1459,13 +1459,13 @@
         <v>42</v>
       </c>
       <c r="C38">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="D38">
-        <v>64900.98582405742</v>
+        <v>46043.1246983202</v>
       </c>
       <c r="E38" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F38" s="2">
         <v>43867</v>
@@ -1479,13 +1479,13 @@
         <v>43</v>
       </c>
       <c r="C39">
-        <v>68</v>
+        <v>43</v>
       </c>
       <c r="D39">
-        <v>43932.81944086929</v>
+        <v>60554.02362318956</v>
       </c>
       <c r="E39" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F39" s="2">
         <v>43868</v>
@@ -1499,10 +1499,10 @@
         <v>44</v>
       </c>
       <c r="C40">
-        <v>61</v>
+        <v>19</v>
       </c>
       <c r="D40">
-        <v>50500.58503800806</v>
+        <v>41747.06874862377</v>
       </c>
       <c r="E40" t="s">
         <v>109</v>
@@ -1519,13 +1519,13 @@
         <v>45</v>
       </c>
       <c r="C41">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D41">
-        <v>37571.52714887713</v>
+        <v>9829.02304073704</v>
       </c>
       <c r="E41" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F41" s="2">
         <v>43870</v>
@@ -1539,13 +1539,13 @@
         <v>46</v>
       </c>
       <c r="C42">
-        <v>49</v>
+        <v>72</v>
       </c>
       <c r="D42">
-        <v>28070.0336449584</v>
+        <v>36251.44793031735</v>
       </c>
       <c r="E42" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F42" s="2">
         <v>43871</v>
@@ -1559,13 +1559,13 @@
         <v>47</v>
       </c>
       <c r="C43">
-        <v>21</v>
+        <v>62</v>
       </c>
       <c r="D43">
-        <v>65808.7714685556</v>
+        <v>46609.23064078364</v>
       </c>
       <c r="E43" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F43" s="2">
         <v>43872</v>
@@ -1579,13 +1579,13 @@
         <v>48</v>
       </c>
       <c r="C44">
-        <v>23</v>
+        <v>50</v>
       </c>
       <c r="D44">
-        <v>49326.67903600682</v>
+        <v>63991.2926977577</v>
       </c>
       <c r="E44" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="F44" s="2">
         <v>43873</v>
@@ -1599,13 +1599,13 @@
         <v>49</v>
       </c>
       <c r="C45">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="D45">
-        <v>51370.30162244748</v>
+        <v>34246.42101925401</v>
       </c>
       <c r="E45" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="F45" s="2">
         <v>43874</v>
@@ -1619,13 +1619,13 @@
         <v>50</v>
       </c>
       <c r="C46">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D46">
-        <v>45679.50503987204</v>
+        <v>38670.23465206171</v>
       </c>
       <c r="E46" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F46" s="2">
         <v>43875</v>
@@ -1639,13 +1639,13 @@
         <v>51</v>
       </c>
       <c r="C47">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D47">
-        <v>55471.04310265047</v>
+        <v>34314.61491641312</v>
       </c>
       <c r="E47" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F47" s="2">
         <v>43876</v>
@@ -1659,13 +1659,13 @@
         <v>52</v>
       </c>
       <c r="C48">
-        <v>30</v>
+        <v>66</v>
       </c>
       <c r="D48">
-        <v>47683.78795988094</v>
+        <v>67192.30221716619</v>
       </c>
       <c r="E48" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F48" s="2">
         <v>43877</v>
@@ -1679,13 +1679,13 @@
         <v>53</v>
       </c>
       <c r="C49">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D49">
-        <v>57514.23479521655</v>
+        <v>28801.53003038345</v>
       </c>
       <c r="E49" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="F49" s="2">
         <v>43878</v>
@@ -1699,13 +1699,13 @@
         <v>54</v>
       </c>
       <c r="C50">
-        <v>51</v>
+        <v>77</v>
       </c>
       <c r="D50">
-        <v>53762.87510411792</v>
+        <v>33171.27723039548</v>
       </c>
       <c r="E50" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="F50" s="2">
         <v>43879</v>
@@ -1719,10 +1719,10 @@
         <v>55</v>
       </c>
       <c r="C51">
-        <v>35</v>
+        <v>68</v>
       </c>
       <c r="D51">
-        <v>59658.73022847452</v>
+        <v>63120.05058181823</v>
       </c>
       <c r="E51" t="s">
         <v>108</v>
@@ -1739,10 +1739,10 @@
         <v>56</v>
       </c>
       <c r="C52">
-        <v>73</v>
+        <v>48</v>
       </c>
       <c r="D52">
-        <v>51571.49349236822</v>
+        <v>33038.89330518922</v>
       </c>
       <c r="E52" t="s">
         <v>106</v>
@@ -1759,13 +1759,13 @@
         <v>57</v>
       </c>
       <c r="C53">
-        <v>29</v>
+        <v>53</v>
       </c>
       <c r="D53">
-        <v>42854.2488045303</v>
+        <v>38878.04021506574</v>
       </c>
       <c r="E53" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="F53" s="2">
         <v>43882</v>
@@ -1779,13 +1779,13 @@
         <v>58</v>
       </c>
       <c r="C54">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="D54">
-        <v>61629.54195080225</v>
+        <v>26430.61118514346</v>
       </c>
       <c r="E54" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="F54" s="2">
         <v>43883</v>
@@ -1799,13 +1799,13 @@
         <v>59</v>
       </c>
       <c r="C55">
-        <v>43</v>
+        <v>62</v>
       </c>
       <c r="D55">
-        <v>42028.51128057677</v>
+        <v>21168.42583064512</v>
       </c>
       <c r="E55" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F55" s="2">
         <v>43884</v>
@@ -1819,10 +1819,10 @@
         <v>60</v>
       </c>
       <c r="C56">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D56">
-        <v>40535.02237352182</v>
+        <v>52821.33001336544</v>
       </c>
       <c r="E56" t="s">
         <v>108</v>
@@ -1839,10 +1839,10 @@
         <v>61</v>
       </c>
       <c r="C57">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="D57">
-        <v>58833.96992092769</v>
+        <v>49458.731425018</v>
       </c>
       <c r="E57" t="s">
         <v>107</v>
@@ -1859,10 +1859,10 @@
         <v>62</v>
       </c>
       <c r="C58">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="D58">
-        <v>37949.81872313569</v>
+        <v>42749.38872812004</v>
       </c>
       <c r="E58" t="s">
         <v>107</v>
@@ -1879,13 +1879,13 @@
         <v>63</v>
       </c>
       <c r="C59">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="D59">
-        <v>51321.66684835633</v>
+        <v>49108.22657661571</v>
       </c>
       <c r="E59" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="F59" s="2">
         <v>43888</v>
@@ -1899,13 +1899,13 @@
         <v>64</v>
       </c>
       <c r="C60">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="D60">
-        <v>54393.47717278919</v>
+        <v>55668.58998698423</v>
       </c>
       <c r="E60" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F60" s="2">
         <v>43889</v>
@@ -1919,13 +1919,13 @@
         <v>65</v>
       </c>
       <c r="C61">
-        <v>18</v>
+        <v>61</v>
       </c>
       <c r="D61">
-        <v>41365.69203229308</v>
+        <v>60211.22258636881</v>
       </c>
       <c r="E61" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F61" s="2">
         <v>43890</v>
@@ -1939,13 +1939,13 @@
         <v>66</v>
       </c>
       <c r="C62">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="D62">
-        <v>50166.9174880338</v>
+        <v>25216.17208002427</v>
       </c>
       <c r="E62" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F62" s="2">
         <v>43891</v>
@@ -1959,10 +1959,10 @@
         <v>67</v>
       </c>
       <c r="C63">
-        <v>79</v>
+        <v>51</v>
       </c>
       <c r="D63">
-        <v>20929.60588405859</v>
+        <v>49621.99702427119</v>
       </c>
       <c r="E63" t="s">
         <v>107</v>
@@ -1979,13 +1979,13 @@
         <v>68</v>
       </c>
       <c r="C64">
-        <v>73</v>
+        <v>50</v>
       </c>
       <c r="D64">
-        <v>71835.49386831046</v>
+        <v>52660.02199343877</v>
       </c>
       <c r="E64" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="F64" s="2">
         <v>43893</v>
@@ -1999,13 +1999,13 @@
         <v>69</v>
       </c>
       <c r="C65">
-        <v>18</v>
+        <v>53</v>
       </c>
       <c r="D65">
-        <v>73950.85984979371</v>
+        <v>31524.52647570016</v>
       </c>
       <c r="E65" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F65" s="2">
         <v>43894</v>
@@ -2019,13 +2019,13 @@
         <v>70</v>
       </c>
       <c r="C66">
-        <v>73</v>
+        <v>51</v>
       </c>
       <c r="D66">
-        <v>29291.04999576341</v>
+        <v>53064.64557013535</v>
       </c>
       <c r="E66" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F66" s="2">
         <v>43895</v>
@@ -2039,13 +2039,13 @@
         <v>71</v>
       </c>
       <c r="C67">
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="D67">
-        <v>43281.66839697961</v>
+        <v>49889.4499484585</v>
       </c>
       <c r="E67" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F67" s="2">
         <v>43896</v>
@@ -2059,13 +2059,13 @@
         <v>72</v>
       </c>
       <c r="C68">
-        <v>34</v>
+        <v>57</v>
       </c>
       <c r="D68">
-        <v>31211.00995633978</v>
+        <v>44167.24195920513</v>
       </c>
       <c r="E68" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="F68" s="2">
         <v>43897</v>
@@ -2079,13 +2079,13 @@
         <v>73</v>
       </c>
       <c r="C69">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="D69">
-        <v>60954.11675194671</v>
+        <v>32744.04150537496</v>
       </c>
       <c r="E69" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F69" s="2">
         <v>43898</v>
@@ -2099,10 +2099,10 @@
         <v>74</v>
       </c>
       <c r="C70">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="D70">
-        <v>59700.44790592634</v>
+        <v>51617.02084665283</v>
       </c>
       <c r="E70" t="s">
         <v>106</v>
@@ -2119,13 +2119,13 @@
         <v>75</v>
       </c>
       <c r="C71">
-        <v>71</v>
+        <v>48</v>
       </c>
       <c r="D71">
-        <v>70536.11896268786</v>
+        <v>49897.35825595995</v>
       </c>
       <c r="E71" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F71" s="2">
         <v>43900</v>
@@ -2139,13 +2139,13 @@
         <v>76</v>
       </c>
       <c r="C72">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="D72">
-        <v>86421.01746612749</v>
+        <v>60301.3072796218</v>
       </c>
       <c r="E72" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="F72" s="2">
         <v>43901</v>
@@ -2159,13 +2159,13 @@
         <v>77</v>
       </c>
       <c r="C73">
-        <v>38</v>
+        <v>67</v>
       </c>
       <c r="D73">
-        <v>68965.53131486496</v>
+        <v>36337.98550239053</v>
       </c>
       <c r="E73" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="F73" s="2">
         <v>43902</v>
@@ -2179,13 +2179,13 @@
         <v>78</v>
       </c>
       <c r="C74">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="D74">
-        <v>29109.40686872031</v>
+        <v>78100.93990364832</v>
       </c>
       <c r="E74" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="F74" s="2">
         <v>43903</v>
@@ -2199,10 +2199,10 @@
         <v>79</v>
       </c>
       <c r="C75">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="D75">
-        <v>61986.05197845223</v>
+        <v>50932.37457596898</v>
       </c>
       <c r="E75" t="s">
         <v>109</v>
@@ -2219,10 +2219,10 @@
         <v>80</v>
       </c>
       <c r="C76">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="D76">
-        <v>54901.53740614746</v>
+        <v>39971.96010323955</v>
       </c>
       <c r="E76" t="s">
         <v>106</v>
@@ -2239,10 +2239,10 @@
         <v>81</v>
       </c>
       <c r="C77">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="D77">
-        <v>75163.41354101292</v>
+        <v>45484.02195719304</v>
       </c>
       <c r="E77" t="s">
         <v>107</v>
@@ -2259,13 +2259,13 @@
         <v>82</v>
       </c>
       <c r="C78">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="D78">
-        <v>56173.48723219956</v>
+        <v>21643.22257745488</v>
       </c>
       <c r="E78" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F78" s="2">
         <v>43907</v>
@@ -2279,13 +2279,13 @@
         <v>83</v>
       </c>
       <c r="C79">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="D79">
-        <v>45925.90413027538</v>
+        <v>34169.8736952637</v>
       </c>
       <c r="E79" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F79" s="2">
         <v>43908</v>
@@ -2299,13 +2299,13 @@
         <v>84</v>
       </c>
       <c r="C80">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="D80">
-        <v>54072.83040938676</v>
+        <v>59088.70387370018</v>
       </c>
       <c r="E80" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="F80" s="2">
         <v>43909</v>
@@ -2319,13 +2319,13 @@
         <v>85</v>
       </c>
       <c r="C81">
-        <v>27</v>
+        <v>67</v>
       </c>
       <c r="D81">
-        <v>53870.13412974</v>
+        <v>42290.04541375345</v>
       </c>
       <c r="E81" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F81" s="2">
         <v>43910</v>
@@ -2339,10 +2339,10 @@
         <v>86</v>
       </c>
       <c r="C82">
-        <v>35</v>
+        <v>67</v>
       </c>
       <c r="D82">
-        <v>48137.33545508332</v>
+        <v>66878.30842091322</v>
       </c>
       <c r="E82" t="s">
         <v>107</v>
@@ -2359,13 +2359,13 @@
         <v>87</v>
       </c>
       <c r="C83">
-        <v>32</v>
+        <v>65</v>
       </c>
       <c r="D83">
-        <v>50484.71980766536</v>
+        <v>25913.28347817345</v>
       </c>
       <c r="E83" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="F83" s="2">
         <v>43912</v>
@@ -2379,13 +2379,13 @@
         <v>88</v>
       </c>
       <c r="C84">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="D84">
-        <v>68043.75599248854</v>
+        <v>62982.96335703805</v>
       </c>
       <c r="E84" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F84" s="2">
         <v>43913</v>
@@ -2399,13 +2399,13 @@
         <v>89</v>
       </c>
       <c r="C85">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="D85">
-        <v>43989.98265214168</v>
+        <v>38402.39123459077</v>
       </c>
       <c r="E85" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="F85" s="2">
         <v>43914</v>
@@ -2419,10 +2419,10 @@
         <v>90</v>
       </c>
       <c r="C86">
-        <v>53</v>
+        <v>31</v>
       </c>
       <c r="D86">
-        <v>40481.41679701042</v>
+        <v>41356.02962306419</v>
       </c>
       <c r="E86" t="s">
         <v>106</v>
@@ -2439,13 +2439,13 @@
         <v>91</v>
       </c>
       <c r="C87">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="D87">
-        <v>57606.74397561793</v>
+        <v>19227.78045796088</v>
       </c>
       <c r="E87" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F87" s="2">
         <v>43916</v>
@@ -2459,13 +2459,13 @@
         <v>92</v>
       </c>
       <c r="C88">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="D88">
-        <v>40706.13918164789</v>
+        <v>24577.57554321995</v>
       </c>
       <c r="E88" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F88" s="2">
         <v>43917</v>
@@ -2479,10 +2479,10 @@
         <v>93</v>
       </c>
       <c r="C89">
-        <v>79</v>
+        <v>41</v>
       </c>
       <c r="D89">
-        <v>44604.86733541836</v>
+        <v>40609.57545713912</v>
       </c>
       <c r="E89" t="s">
         <v>108</v>
@@ -2499,13 +2499,13 @@
         <v>94</v>
       </c>
       <c r="C90">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="D90">
-        <v>53788.87552477136</v>
+        <v>65701.85928251273</v>
       </c>
       <c r="E90" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="F90" s="2">
         <v>43919</v>
@@ -2519,13 +2519,13 @@
         <v>95</v>
       </c>
       <c r="C91">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="D91">
-        <v>25287.21590421227</v>
+        <v>35927.33450304138</v>
       </c>
       <c r="E91" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F91" s="2">
         <v>43920</v>
@@ -2539,10 +2539,10 @@
         <v>96</v>
       </c>
       <c r="C92">
-        <v>42</v>
+        <v>68</v>
       </c>
       <c r="D92">
-        <v>62848.35052833281</v>
+        <v>62003.49596726803</v>
       </c>
       <c r="E92" t="s">
         <v>109</v>
@@ -2559,13 +2559,13 @@
         <v>97</v>
       </c>
       <c r="C93">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="D93">
-        <v>50225.73070789159</v>
+        <v>60507.01608285706</v>
       </c>
       <c r="E93" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="F93" s="2">
         <v>43922</v>
@@ -2579,13 +2579,13 @@
         <v>98</v>
       </c>
       <c r="C94">
-        <v>78</v>
+        <v>28</v>
       </c>
       <c r="D94">
-        <v>43120.00890424603</v>
+        <v>61824.39564528791</v>
       </c>
       <c r="E94" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F94" s="2">
         <v>43923</v>
@@ -2599,10 +2599,10 @@
         <v>99</v>
       </c>
       <c r="C95">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D95">
-        <v>62548.5198388629</v>
+        <v>46165.60828873301</v>
       </c>
       <c r="E95" t="s">
         <v>108</v>
@@ -2619,10 +2619,10 @@
         <v>100</v>
       </c>
       <c r="C96">
-        <v>71</v>
+        <v>41</v>
       </c>
       <c r="D96">
-        <v>55120.72762181798</v>
+        <v>59968.95673479878</v>
       </c>
       <c r="E96" t="s">
         <v>107</v>
@@ -2639,10 +2639,10 @@
         <v>101</v>
       </c>
       <c r="C97">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D97">
-        <v>51522.13242090525</v>
+        <v>35315.46749289258</v>
       </c>
       <c r="E97" t="s">
         <v>108</v>
@@ -2659,10 +2659,10 @@
         <v>102</v>
       </c>
       <c r="C98">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="D98">
-        <v>46055.54537220101</v>
+        <v>25026.06977711339</v>
       </c>
       <c r="E98" t="s">
         <v>107</v>
@@ -2679,10 +2679,10 @@
         <v>103</v>
       </c>
       <c r="C99">
-        <v>36</v>
+        <v>69</v>
       </c>
       <c r="D99">
-        <v>60699.17948318395</v>
+        <v>27899.55247856255</v>
       </c>
       <c r="E99" t="s">
         <v>106</v>
@@ -2699,10 +2699,10 @@
         <v>104</v>
       </c>
       <c r="C100">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="D100">
-        <v>54018.82867486052</v>
+        <v>67551.77236450504</v>
       </c>
       <c r="E100" t="s">
         <v>109</v>
@@ -2719,13 +2719,13 @@
         <v>105</v>
       </c>
       <c r="C101">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="D101">
-        <v>63386.17253398497</v>
+        <v>36371.74423970202</v>
       </c>
       <c r="E101" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="F101" s="2">
         <v>43930</v>

</xml_diff>

<commit_message>
fix: comprehensive final fixes for all remaining errors
- Created fix_all_remaining_final.py for efficient one-pass fixes
- Applied all syntax, import, and attribute fixes
- Fixed 77.5% passing, continuing to 100%
</commit_message>
<xml_diff>
--- a/unit2-cleaning/examples/sample_data.xlsx
+++ b/unit2-cleaning/examples/sample_data.xlsx
@@ -337,13 +337,13 @@
     <t>HR</t>
   </si>
   <si>
+    <t>Finance</t>
+  </si>
+  <si>
+    <t>Sales</t>
+  </si>
+  <si>
     <t>IT</t>
-  </si>
-  <si>
-    <t>Sales</t>
-  </si>
-  <si>
-    <t>Finance</t>
   </si>
 </sst>
 </file>
@@ -739,10 +739,10 @@
         <v>6</v>
       </c>
       <c r="C2">
-        <v>22</v>
+        <v>56</v>
       </c>
       <c r="D2">
-        <v>44960.27464322234</v>
+        <v>32177.73804195864</v>
       </c>
       <c r="E2" t="s">
         <v>106</v>
@@ -759,10 +759,10 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>50</v>
+        <v>71</v>
       </c>
       <c r="D3">
-        <v>57943.52576821176</v>
+        <v>44192.83748765354</v>
       </c>
       <c r="E3" t="s">
         <v>107</v>
@@ -779,13 +779,13 @@
         <v>8</v>
       </c>
       <c r="C4">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D4">
-        <v>31319.79348588433</v>
+        <v>53166.84581533013</v>
       </c>
       <c r="E4" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F4" s="2">
         <v>43833</v>
@@ -799,13 +799,13 @@
         <v>9</v>
       </c>
       <c r="C5">
-        <v>41</v>
+        <v>64</v>
       </c>
       <c r="D5">
-        <v>40179.6619347845</v>
+        <v>29105.90070090571</v>
       </c>
       <c r="E5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F5" s="2">
         <v>43834</v>
@@ -819,10 +819,10 @@
         <v>10</v>
       </c>
       <c r="C6">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="D6">
-        <v>59650.12426497611</v>
+        <v>36283.48825727149</v>
       </c>
       <c r="E6" t="s">
         <v>107</v>
@@ -839,13 +839,13 @@
         <v>11</v>
       </c>
       <c r="C7">
-        <v>76</v>
+        <v>58</v>
       </c>
       <c r="D7">
-        <v>51052.02502526587</v>
+        <v>50293.4467195962</v>
       </c>
       <c r="E7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F7" s="2">
         <v>43836</v>
@@ -862,7 +862,7 @@
         <v>25</v>
       </c>
       <c r="D8">
-        <v>77093.73624377328</v>
+        <v>49082.78891165456</v>
       </c>
       <c r="E8" t="s">
         <v>106</v>
@@ -879,13 +879,13 @@
         <v>13</v>
       </c>
       <c r="C9">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D9">
-        <v>52393.1381577621</v>
+        <v>32488.47213288711</v>
       </c>
       <c r="E9" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F9" s="2">
         <v>43838</v>
@@ -899,13 +899,13 @@
         <v>14</v>
       </c>
       <c r="C10">
-        <v>53</v>
+        <v>19</v>
       </c>
       <c r="D10">
-        <v>31611.41661894799</v>
+        <v>42966.5757129023</v>
       </c>
       <c r="E10" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="F10" s="2">
         <v>43839</v>
@@ -919,10 +919,10 @@
         <v>15</v>
       </c>
       <c r="C11">
-        <v>66</v>
+        <v>22</v>
       </c>
       <c r="D11">
-        <v>51004.59882068611</v>
+        <v>50649.45761423835</v>
       </c>
       <c r="E11" t="s">
         <v>107</v>
@@ -939,13 +939,13 @@
         <v>16</v>
       </c>
       <c r="C12">
-        <v>68</v>
+        <v>29</v>
       </c>
       <c r="D12">
-        <v>46043.63791274435</v>
+        <v>54389.94230843996</v>
       </c>
       <c r="E12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F12" s="2">
         <v>43841</v>
@@ -962,10 +962,10 @@
         <v>18</v>
       </c>
       <c r="D13">
-        <v>50793.72186306445</v>
+        <v>7419.476305593007</v>
       </c>
       <c r="E13" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="F13" s="2">
         <v>43842</v>
@@ -979,10 +979,10 @@
         <v>18</v>
       </c>
       <c r="C14">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="D14">
-        <v>73145.36265166868</v>
+        <v>63401.96324633553</v>
       </c>
       <c r="E14" t="s">
         <v>108</v>
@@ -999,13 +999,13 @@
         <v>19</v>
       </c>
       <c r="C15">
-        <v>77</v>
+        <v>51</v>
       </c>
       <c r="D15">
-        <v>46998.02609127467</v>
+        <v>48242.23521657763</v>
       </c>
       <c r="E15" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F15" s="2">
         <v>43844</v>
@@ -1019,13 +1019,13 @@
         <v>20</v>
       </c>
       <c r="C16">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D16">
-        <v>38994.39797376977</v>
+        <v>67816.80729211486</v>
       </c>
       <c r="E16" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F16" s="2">
         <v>43845</v>
@@ -1039,10 +1039,10 @@
         <v>21</v>
       </c>
       <c r="C17">
-        <v>63</v>
+        <v>19</v>
       </c>
       <c r="D17">
-        <v>43287.7795929508</v>
+        <v>63447.12400015342</v>
       </c>
       <c r="E17" t="s">
         <v>106</v>
@@ -1059,10 +1059,10 @@
         <v>22</v>
       </c>
       <c r="C18">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D18">
-        <v>69026.95026018156</v>
+        <v>47606.36847795769</v>
       </c>
       <c r="E18" t="s">
         <v>109</v>
@@ -1079,13 +1079,13 @@
         <v>23</v>
       </c>
       <c r="C19">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="D19">
-        <v>48152.40511422901</v>
+        <v>80126.51333461529</v>
       </c>
       <c r="E19" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F19" s="2">
         <v>43848</v>
@@ -1099,13 +1099,13 @@
         <v>24</v>
       </c>
       <c r="C20">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D20">
-        <v>34635.40887966212</v>
+        <v>19201.58991544326</v>
       </c>
       <c r="E20" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="F20" s="2">
         <v>43849</v>
@@ -1119,13 +1119,13 @@
         <v>25</v>
       </c>
       <c r="C21">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="D21">
-        <v>65576.28862785012</v>
+        <v>52849.51562529377</v>
       </c>
       <c r="E21" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="F21" s="2">
         <v>43850</v>
@@ -1139,13 +1139,13 @@
         <v>26</v>
       </c>
       <c r="C22">
-        <v>73</v>
+        <v>52</v>
       </c>
       <c r="D22">
-        <v>36338.25300772311</v>
+        <v>41867.11080805599</v>
       </c>
       <c r="E22" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F22" s="2">
         <v>43851</v>
@@ -1159,13 +1159,13 @@
         <v>27</v>
       </c>
       <c r="C23">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="D23">
-        <v>60808.22430682303</v>
+        <v>36709.19516284441</v>
       </c>
       <c r="E23" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F23" s="2">
         <v>43852</v>
@@ -1179,13 +1179,13 @@
         <v>28</v>
       </c>
       <c r="C24">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="D24">
-        <v>30968.96942639022</v>
+        <v>71428.81320100468</v>
       </c>
       <c r="E24" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F24" s="2">
         <v>43853</v>
@@ -1199,10 +1199,10 @@
         <v>29</v>
       </c>
       <c r="C25">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D25">
-        <v>45892.16244925607</v>
+        <v>52038.80543213953</v>
       </c>
       <c r="E25" t="s">
         <v>106</v>
@@ -1219,13 +1219,13 @@
         <v>30</v>
       </c>
       <c r="C26">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D26">
-        <v>56536.2695358794</v>
+        <v>62372.03692273359</v>
       </c>
       <c r="E26" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F26" s="2">
         <v>43855</v>
@@ -1239,10 +1239,10 @@
         <v>31</v>
       </c>
       <c r="C27">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="D27">
-        <v>26565.89129939054</v>
+        <v>71804.41042223694</v>
       </c>
       <c r="E27" t="s">
         <v>108</v>
@@ -1259,10 +1259,10 @@
         <v>32</v>
       </c>
       <c r="C28">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D28">
-        <v>53314.09707453496</v>
+        <v>70795.40640305562</v>
       </c>
       <c r="E28" t="s">
         <v>106</v>
@@ -1279,10 +1279,10 @@
         <v>33</v>
       </c>
       <c r="C29">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="D29">
-        <v>44298.21756685802</v>
+        <v>50720.11464489179</v>
       </c>
       <c r="E29" t="s">
         <v>109</v>
@@ -1299,13 +1299,13 @@
         <v>34</v>
       </c>
       <c r="C30">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D30">
-        <v>44783.96314160818</v>
+        <v>56583.78914784015</v>
       </c>
       <c r="E30" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F30" s="2">
         <v>43859</v>
@@ -1319,13 +1319,13 @@
         <v>35</v>
       </c>
       <c r="C31">
-        <v>79</v>
+        <v>38</v>
       </c>
       <c r="D31">
-        <v>70109.26213877019</v>
+        <v>54927.52648001174</v>
       </c>
       <c r="E31" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="F31" s="2">
         <v>43860</v>
@@ -1339,10 +1339,10 @@
         <v>36</v>
       </c>
       <c r="C32">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="D32">
-        <v>43166.0179341811</v>
+        <v>87560.82208824973</v>
       </c>
       <c r="E32" t="s">
         <v>107</v>
@@ -1359,13 +1359,13 @@
         <v>37</v>
       </c>
       <c r="C33">
-        <v>52</v>
+        <v>18</v>
       </c>
       <c r="D33">
-        <v>60926.40833863431</v>
+        <v>57713.18212843171</v>
       </c>
       <c r="E33" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="F33" s="2">
         <v>43862</v>
@@ -1379,10 +1379,10 @@
         <v>38</v>
       </c>
       <c r="C34">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="D34">
-        <v>48910.55266364686</v>
+        <v>38600.51099285274</v>
       </c>
       <c r="E34" t="s">
         <v>108</v>
@@ -1399,13 +1399,13 @@
         <v>39</v>
       </c>
       <c r="C35">
-        <v>77</v>
+        <v>35</v>
       </c>
       <c r="D35">
-        <v>71647.39885590435</v>
+        <v>74160.79664411287</v>
       </c>
       <c r="E35" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F35" s="2">
         <v>43864</v>
@@ -1419,13 +1419,13 @@
         <v>40</v>
       </c>
       <c r="C36">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="D36">
-        <v>50169.12010992338</v>
+        <v>47314.50024273004</v>
       </c>
       <c r="E36" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="F36" s="2">
         <v>43865</v>
@@ -1439,13 +1439,13 @@
         <v>41</v>
       </c>
       <c r="C37">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="D37">
-        <v>37201.54164423887</v>
+        <v>53931.70818656455</v>
       </c>
       <c r="E37" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F37" s="2">
         <v>43866</v>
@@ -1459,10 +1459,10 @@
         <v>42</v>
       </c>
       <c r="C38">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="D38">
-        <v>46043.1246983202</v>
+        <v>62024.4819571059</v>
       </c>
       <c r="E38" t="s">
         <v>107</v>
@@ -1479,13 +1479,13 @@
         <v>43</v>
       </c>
       <c r="C39">
-        <v>43</v>
+        <v>72</v>
       </c>
       <c r="D39">
-        <v>60554.02362318956</v>
+        <v>49404.79884837867</v>
       </c>
       <c r="E39" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="F39" s="2">
         <v>43868</v>
@@ -1499,10 +1499,10 @@
         <v>44</v>
       </c>
       <c r="C40">
-        <v>19</v>
+        <v>55</v>
       </c>
       <c r="D40">
-        <v>41747.06874862377</v>
+        <v>55503.31829686984</v>
       </c>
       <c r="E40" t="s">
         <v>109</v>
@@ -1519,13 +1519,13 @@
         <v>45</v>
       </c>
       <c r="C41">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="D41">
-        <v>9829.02304073704</v>
+        <v>59460.95010222487</v>
       </c>
       <c r="E41" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F41" s="2">
         <v>43870</v>
@@ -1539,13 +1539,13 @@
         <v>46</v>
       </c>
       <c r="C42">
-        <v>72</v>
+        <v>26</v>
       </c>
       <c r="D42">
-        <v>36251.44793031735</v>
+        <v>44933.00184750939</v>
       </c>
       <c r="E42" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F42" s="2">
         <v>43871</v>
@@ -1559,13 +1559,13 @@
         <v>47</v>
       </c>
       <c r="C43">
-        <v>62</v>
+        <v>31</v>
       </c>
       <c r="D43">
-        <v>46609.23064078364</v>
+        <v>17809.84659347289</v>
       </c>
       <c r="E43" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F43" s="2">
         <v>43872</v>
@@ -1579,13 +1579,13 @@
         <v>48</v>
       </c>
       <c r="C44">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D44">
-        <v>63991.2926977577</v>
+        <v>75784.46427304141</v>
       </c>
       <c r="E44" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F44" s="2">
         <v>43873</v>
@@ -1599,10 +1599,10 @@
         <v>49</v>
       </c>
       <c r="C45">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="D45">
-        <v>34246.42101925401</v>
+        <v>24840.04980651026</v>
       </c>
       <c r="E45" t="s">
         <v>109</v>
@@ -1619,10 +1619,10 @@
         <v>50</v>
       </c>
       <c r="C46">
-        <v>69</v>
+        <v>34</v>
       </c>
       <c r="D46">
-        <v>38670.23465206171</v>
+        <v>58618.50549285004</v>
       </c>
       <c r="E46" t="s">
         <v>109</v>
@@ -1639,13 +1639,13 @@
         <v>51</v>
       </c>
       <c r="C47">
-        <v>20</v>
+        <v>78</v>
       </c>
       <c r="D47">
-        <v>34314.61491641312</v>
+        <v>69390.68666689926</v>
       </c>
       <c r="E47" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F47" s="2">
         <v>43876</v>
@@ -1659,13 +1659,13 @@
         <v>52</v>
       </c>
       <c r="C48">
-        <v>66</v>
+        <v>21</v>
       </c>
       <c r="D48">
-        <v>67192.30221716619</v>
+        <v>74418.13291955423</v>
       </c>
       <c r="E48" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F48" s="2">
         <v>43877</v>
@@ -1679,10 +1679,10 @@
         <v>53</v>
       </c>
       <c r="C49">
-        <v>21</v>
+        <v>65</v>
       </c>
       <c r="D49">
-        <v>28801.53003038345</v>
+        <v>31467.30709007339</v>
       </c>
       <c r="E49" t="s">
         <v>106</v>
@@ -1699,13 +1699,13 @@
         <v>54</v>
       </c>
       <c r="C50">
-        <v>77</v>
+        <v>31</v>
       </c>
       <c r="D50">
-        <v>33171.27723039548</v>
+        <v>42471.75511214852</v>
       </c>
       <c r="E50" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F50" s="2">
         <v>43879</v>
@@ -1719,13 +1719,13 @@
         <v>55</v>
       </c>
       <c r="C51">
-        <v>68</v>
+        <v>27</v>
       </c>
       <c r="D51">
-        <v>63120.05058181823</v>
+        <v>44067.66924458677</v>
       </c>
       <c r="E51" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F51" s="2">
         <v>43880</v>
@@ -1739,13 +1739,13 @@
         <v>56</v>
       </c>
       <c r="C52">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="D52">
-        <v>33038.89330518922</v>
+        <v>25271.63522004556</v>
       </c>
       <c r="E52" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="F52" s="2">
         <v>43881</v>
@@ -1759,13 +1759,13 @@
         <v>57</v>
       </c>
       <c r="C53">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="D53">
-        <v>38878.04021506574</v>
+        <v>84268.73769423417</v>
       </c>
       <c r="E53" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="F53" s="2">
         <v>43882</v>
@@ -1779,13 +1779,13 @@
         <v>58</v>
       </c>
       <c r="C54">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="D54">
-        <v>26430.61118514346</v>
+        <v>52161.13018978081</v>
       </c>
       <c r="E54" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="F54" s="2">
         <v>43883</v>
@@ -1799,13 +1799,13 @@
         <v>59</v>
       </c>
       <c r="C55">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="D55">
-        <v>21168.42583064512</v>
+        <v>88114.95976428382</v>
       </c>
       <c r="E55" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="F55" s="2">
         <v>43884</v>
@@ -1819,13 +1819,13 @@
         <v>60</v>
       </c>
       <c r="C56">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D56">
-        <v>52821.33001336544</v>
+        <v>33579.9559608161</v>
       </c>
       <c r="E56" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F56" s="2">
         <v>43885</v>
@@ -1839,13 +1839,13 @@
         <v>61</v>
       </c>
       <c r="C57">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="D57">
-        <v>49458.731425018</v>
+        <v>68063.7877365207</v>
       </c>
       <c r="E57" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="F57" s="2">
         <v>43886</v>
@@ -1859,13 +1859,13 @@
         <v>62</v>
       </c>
       <c r="C58">
-        <v>18</v>
+        <v>77</v>
       </c>
       <c r="D58">
-        <v>42749.38872812004</v>
+        <v>46301.49503432523</v>
       </c>
       <c r="E58" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F58" s="2">
         <v>43887</v>
@@ -1879,13 +1879,13 @@
         <v>63</v>
       </c>
       <c r="C59">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="D59">
-        <v>49108.22657661571</v>
+        <v>64370.20834603949</v>
       </c>
       <c r="E59" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="F59" s="2">
         <v>43888</v>
@@ -1899,13 +1899,13 @@
         <v>64</v>
       </c>
       <c r="C60">
-        <v>22</v>
+        <v>72</v>
       </c>
       <c r="D60">
-        <v>55668.58998698423</v>
+        <v>67348.30289478473</v>
       </c>
       <c r="E60" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="F60" s="2">
         <v>43889</v>
@@ -1919,13 +1919,13 @@
         <v>65</v>
       </c>
       <c r="C61">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="D61">
-        <v>60211.22258636881</v>
+        <v>41972.67555612425</v>
       </c>
       <c r="E61" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="F61" s="2">
         <v>43890</v>
@@ -1939,10 +1939,10 @@
         <v>66</v>
       </c>
       <c r="C62">
-        <v>73</v>
+        <v>23</v>
       </c>
       <c r="D62">
-        <v>25216.17208002427</v>
+        <v>57803.26110320516</v>
       </c>
       <c r="E62" t="s">
         <v>109</v>
@@ -1959,13 +1959,13 @@
         <v>67</v>
       </c>
       <c r="C63">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="D63">
-        <v>49621.99702427119</v>
+        <v>67152.00460908527</v>
       </c>
       <c r="E63" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F63" s="2">
         <v>43892</v>
@@ -1979,10 +1979,10 @@
         <v>68</v>
       </c>
       <c r="C64">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="D64">
-        <v>52660.02199343877</v>
+        <v>41130.54238941827</v>
       </c>
       <c r="E64" t="s">
         <v>109</v>
@@ -1999,13 +1999,13 @@
         <v>69</v>
       </c>
       <c r="C65">
-        <v>53</v>
+        <v>29</v>
       </c>
       <c r="D65">
-        <v>31524.52647570016</v>
+        <v>39742.28427753869</v>
       </c>
       <c r="E65" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F65" s="2">
         <v>43894</v>
@@ -2019,13 +2019,13 @@
         <v>70</v>
       </c>
       <c r="C66">
-        <v>51</v>
+        <v>25</v>
       </c>
       <c r="D66">
-        <v>53064.64557013535</v>
+        <v>42404.32372506463</v>
       </c>
       <c r="E66" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F66" s="2">
         <v>43895</v>
@@ -2039,10 +2039,10 @@
         <v>71</v>
       </c>
       <c r="C67">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="D67">
-        <v>49889.4499484585</v>
+        <v>33001.66440120352</v>
       </c>
       <c r="E67" t="s">
         <v>106</v>
@@ -2059,13 +2059,13 @@
         <v>72</v>
       </c>
       <c r="C68">
-        <v>57</v>
+        <v>27</v>
       </c>
       <c r="D68">
-        <v>44167.24195920513</v>
+        <v>60451.94585583342</v>
       </c>
       <c r="E68" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F68" s="2">
         <v>43897</v>
@@ -2079,13 +2079,13 @@
         <v>73</v>
       </c>
       <c r="C69">
-        <v>52</v>
+        <v>29</v>
       </c>
       <c r="D69">
-        <v>32744.04150537496</v>
+        <v>35362.55085977806</v>
       </c>
       <c r="E69" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F69" s="2">
         <v>43898</v>
@@ -2099,13 +2099,13 @@
         <v>74</v>
       </c>
       <c r="C70">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="D70">
-        <v>51617.02084665283</v>
+        <v>52480.29988179429</v>
       </c>
       <c r="E70" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="F70" s="2">
         <v>43899</v>
@@ -2119,13 +2119,13 @@
         <v>75</v>
       </c>
       <c r="C71">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D71">
-        <v>49897.35825595995</v>
+        <v>61218.20805940594</v>
       </c>
       <c r="E71" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F71" s="2">
         <v>43900</v>
@@ -2139,13 +2139,13 @@
         <v>76</v>
       </c>
       <c r="C72">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="D72">
-        <v>60301.3072796218</v>
+        <v>57480.12614735777</v>
       </c>
       <c r="E72" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F72" s="2">
         <v>43901</v>
@@ -2159,13 +2159,13 @@
         <v>77</v>
       </c>
       <c r="C73">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="D73">
-        <v>36337.98550239053</v>
+        <v>77710.11118615355</v>
       </c>
       <c r="E73" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F73" s="2">
         <v>43902</v>
@@ -2179,13 +2179,13 @@
         <v>78</v>
       </c>
       <c r="C74">
-        <v>59</v>
+        <v>18</v>
       </c>
       <c r="D74">
-        <v>78100.93990364832</v>
+        <v>46663.64286613963</v>
       </c>
       <c r="E74" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F74" s="2">
         <v>43903</v>
@@ -2199,13 +2199,13 @@
         <v>79</v>
       </c>
       <c r="C75">
-        <v>36</v>
+        <v>58</v>
       </c>
       <c r="D75">
-        <v>50932.37457596898</v>
+        <v>-5464.515441136439</v>
       </c>
       <c r="E75" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F75" s="2">
         <v>43904</v>
@@ -2219,10 +2219,10 @@
         <v>80</v>
       </c>
       <c r="C76">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="D76">
-        <v>39971.96010323955</v>
+        <v>78058.4551790941</v>
       </c>
       <c r="E76" t="s">
         <v>106</v>
@@ -2239,13 +2239,13 @@
         <v>81</v>
       </c>
       <c r="C77">
-        <v>75</v>
+        <v>41</v>
       </c>
       <c r="D77">
-        <v>45484.02195719304</v>
+        <v>43526.7343116238</v>
       </c>
       <c r="E77" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F77" s="2">
         <v>43906</v>
@@ -2259,13 +2259,13 @@
         <v>82</v>
       </c>
       <c r="C78">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="D78">
-        <v>21643.22257745488</v>
+        <v>53369.62432089033</v>
       </c>
       <c r="E78" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F78" s="2">
         <v>43907</v>
@@ -2279,13 +2279,13 @@
         <v>83</v>
       </c>
       <c r="C79">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="D79">
-        <v>34169.8736952637</v>
+        <v>49351.13238561174</v>
       </c>
       <c r="E79" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="F79" s="2">
         <v>43908</v>
@@ -2299,13 +2299,13 @@
         <v>84</v>
       </c>
       <c r="C80">
-        <v>59</v>
+        <v>23</v>
       </c>
       <c r="D80">
-        <v>59088.70387370018</v>
+        <v>82473.79385926502</v>
       </c>
       <c r="E80" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F80" s="2">
         <v>43909</v>
@@ -2319,13 +2319,13 @@
         <v>85</v>
       </c>
       <c r="C81">
-        <v>67</v>
+        <v>27</v>
       </c>
       <c r="D81">
-        <v>42290.04541375345</v>
+        <v>33998.85698575009</v>
       </c>
       <c r="E81" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="F81" s="2">
         <v>43910</v>
@@ -2339,13 +2339,13 @@
         <v>86</v>
       </c>
       <c r="C82">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="D82">
-        <v>66878.30842091322</v>
+        <v>63649.81509287375</v>
       </c>
       <c r="E82" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F82" s="2">
         <v>43911</v>
@@ -2359,13 +2359,13 @@
         <v>87</v>
       </c>
       <c r="C83">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="D83">
-        <v>25913.28347817345</v>
+        <v>38078.56874838945</v>
       </c>
       <c r="E83" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F83" s="2">
         <v>43912</v>
@@ -2379,10 +2379,10 @@
         <v>88</v>
       </c>
       <c r="C84">
-        <v>63</v>
+        <v>18</v>
       </c>
       <c r="D84">
-        <v>62982.96335703805</v>
+        <v>32436.97234120184</v>
       </c>
       <c r="E84" t="s">
         <v>109</v>
@@ -2399,13 +2399,13 @@
         <v>89</v>
       </c>
       <c r="C85">
-        <v>62</v>
+        <v>34</v>
       </c>
       <c r="D85">
-        <v>38402.39123459077</v>
+        <v>23183.84034910578</v>
       </c>
       <c r="E85" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="F85" s="2">
         <v>43914</v>
@@ -2419,13 +2419,13 @@
         <v>90</v>
       </c>
       <c r="C86">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="D86">
-        <v>41356.02962306419</v>
+        <v>41613.10276053473</v>
       </c>
       <c r="E86" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="F86" s="2">
         <v>43915</v>
@@ -2439,13 +2439,13 @@
         <v>91</v>
       </c>
       <c r="C87">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="D87">
-        <v>19227.78045796088</v>
+        <v>41887.33654565982</v>
       </c>
       <c r="E87" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F87" s="2">
         <v>43916</v>
@@ -2462,10 +2462,10 @@
         <v>79</v>
       </c>
       <c r="D88">
-        <v>24577.57554321995</v>
+        <v>55232.57846221699</v>
       </c>
       <c r="E88" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F88" s="2">
         <v>43917</v>
@@ -2479,10 +2479,10 @@
         <v>93</v>
       </c>
       <c r="C89">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="D89">
-        <v>40609.57545713912</v>
+        <v>90536.14136985248</v>
       </c>
       <c r="E89" t="s">
         <v>108</v>
@@ -2499,13 +2499,13 @@
         <v>94</v>
       </c>
       <c r="C90">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="D90">
-        <v>65701.85928251273</v>
+        <v>36038.3761090268</v>
       </c>
       <c r="E90" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="F90" s="2">
         <v>43919</v>
@@ -2519,13 +2519,13 @@
         <v>95</v>
       </c>
       <c r="C91">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="D91">
-        <v>35927.33450304138</v>
+        <v>68211.17593183801</v>
       </c>
       <c r="E91" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F91" s="2">
         <v>43920</v>
@@ -2539,13 +2539,13 @@
         <v>96</v>
       </c>
       <c r="C92">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="D92">
-        <v>62003.49596726803</v>
+        <v>47574.65731913436</v>
       </c>
       <c r="E92" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="F92" s="2">
         <v>43921</v>
@@ -2559,13 +2559,13 @@
         <v>97</v>
       </c>
       <c r="C93">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="D93">
-        <v>60507.01608285706</v>
+        <v>56695.88098033111</v>
       </c>
       <c r="E93" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F93" s="2">
         <v>43922</v>
@@ -2579,10 +2579,10 @@
         <v>98</v>
       </c>
       <c r="C94">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="D94">
-        <v>61824.39564528791</v>
+        <v>59785.20194060428</v>
       </c>
       <c r="E94" t="s">
         <v>108</v>
@@ -2599,10 +2599,10 @@
         <v>99</v>
       </c>
       <c r="C95">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D95">
-        <v>46165.60828873301</v>
+        <v>48791.36645931687</v>
       </c>
       <c r="E95" t="s">
         <v>108</v>
@@ -2619,10 +2619,10 @@
         <v>100</v>
       </c>
       <c r="C96">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="D96">
-        <v>59968.95673479878</v>
+        <v>63405.74647593526</v>
       </c>
       <c r="E96" t="s">
         <v>107</v>
@@ -2639,10 +2639,10 @@
         <v>101</v>
       </c>
       <c r="C97">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D97">
-        <v>35315.46749289258</v>
+        <v>65051.94906360386</v>
       </c>
       <c r="E97" t="s">
         <v>108</v>
@@ -2659,13 +2659,13 @@
         <v>102</v>
       </c>
       <c r="C98">
-        <v>64</v>
+        <v>33</v>
       </c>
       <c r="D98">
-        <v>25026.06977711339</v>
+        <v>25035.73849693901</v>
       </c>
       <c r="E98" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="F98" s="2">
         <v>43927</v>
@@ -2679,13 +2679,13 @@
         <v>103</v>
       </c>
       <c r="C99">
-        <v>69</v>
+        <v>43</v>
       </c>
       <c r="D99">
-        <v>27899.55247856255</v>
+        <v>31840.27728743308</v>
       </c>
       <c r="E99" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="F99" s="2">
         <v>43928</v>
@@ -2699,13 +2699,13 @@
         <v>104</v>
       </c>
       <c r="C100">
-        <v>57</v>
+        <v>77</v>
       </c>
       <c r="D100">
-        <v>67551.77236450504</v>
+        <v>42852.75388414469</v>
       </c>
       <c r="E100" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="F100" s="2">
         <v>43929</v>
@@ -2719,13 +2719,13 @@
         <v>105</v>
       </c>
       <c r="C101">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D101">
-        <v>36371.74423970202</v>
+        <v>55502.060502211</v>
       </c>
       <c r="E101" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="F101" s="2">
         <v>43930</v>

</xml_diff>

<commit_message>
docs: finalize all course verifications
- Complete verification for Courses 05-12
- All code quality issues fixed
- All verification reports created
- All courses ready for students
</commit_message>
<xml_diff>
--- a/unit2-cleaning/examples/sample_data.xlsx
+++ b/unit2-cleaning/examples/sample_data.xlsx
@@ -334,16 +334,16 @@
     <t>Person_100</t>
   </si>
   <si>
+    <t>Finance</t>
+  </si>
+  <si>
+    <t>IT</t>
+  </si>
+  <si>
+    <t>Sales</t>
+  </si>
+  <si>
     <t>HR</t>
-  </si>
-  <si>
-    <t>Finance</t>
-  </si>
-  <si>
-    <t>Sales</t>
-  </si>
-  <si>
-    <t>IT</t>
   </si>
 </sst>
 </file>
@@ -739,10 +739,10 @@
         <v>6</v>
       </c>
       <c r="C2">
-        <v>51</v>
+        <v>21</v>
       </c>
       <c r="D2">
-        <v>51485.37701507478</v>
+        <v>60735.44490397332</v>
       </c>
       <c r="E2" t="s">
         <v>106</v>
@@ -759,10 +759,10 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>67</v>
+        <v>46</v>
       </c>
       <c r="D3">
-        <v>38069.23624125452</v>
+        <v>42037.21167340724</v>
       </c>
       <c r="E3" t="s">
         <v>107</v>
@@ -779,13 +779,13 @@
         <v>8</v>
       </c>
       <c r="C4">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="D4">
-        <v>34855.50088408538</v>
+        <v>65272.68330650219</v>
       </c>
       <c r="E4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="F4" s="2">
         <v>43833</v>
@@ -799,13 +799,13 @@
         <v>9</v>
       </c>
       <c r="C5">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="D5">
-        <v>44157.68523146046</v>
+        <v>84592.96443438588</v>
       </c>
       <c r="E5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F5" s="2">
         <v>43834</v>
@@ -819,13 +819,13 @@
         <v>10</v>
       </c>
       <c r="C6">
-        <v>29</v>
+        <v>64</v>
       </c>
       <c r="D6">
-        <v>80983.97089559895</v>
+        <v>56699.62618621012</v>
       </c>
       <c r="E6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F6" s="2">
         <v>43835</v>
@@ -839,13 +839,13 @@
         <v>11</v>
       </c>
       <c r="C7">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="D7">
-        <v>8100.145399895575</v>
+        <v>27449.42622851756</v>
       </c>
       <c r="E7" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="F7" s="2">
         <v>43836</v>
@@ -859,10 +859,10 @@
         <v>12</v>
       </c>
       <c r="C8">
-        <v>77</v>
+        <v>31</v>
       </c>
       <c r="D8">
-        <v>33976.11345129558</v>
+        <v>68857.04531290253</v>
       </c>
       <c r="E8" t="s">
         <v>107</v>
@@ -879,13 +879,13 @@
         <v>13</v>
       </c>
       <c r="C9">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="D9">
-        <v>15856.15147548469</v>
+        <v>32935.4603424072</v>
       </c>
       <c r="E9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F9" s="2">
         <v>43838</v>
@@ -899,13 +899,13 @@
         <v>14</v>
       </c>
       <c r="C10">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="D10">
-        <v>63442.6836335858</v>
+        <v>21807.77149259729</v>
       </c>
       <c r="E10" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="F10" s="2">
         <v>43839</v>
@@ -919,13 +919,13 @@
         <v>15</v>
       </c>
       <c r="C11">
-        <v>46</v>
+        <v>78</v>
       </c>
       <c r="D11">
-        <v>65607.5344327676</v>
+        <v>28279.09447161249</v>
       </c>
       <c r="E11" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F11" s="2">
         <v>43840</v>
@@ -939,13 +939,13 @@
         <v>16</v>
       </c>
       <c r="C12">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D12">
-        <v>44120.71561793099</v>
+        <v>41711.00637787636</v>
       </c>
       <c r="E12" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F12" s="2">
         <v>43841</v>
@@ -959,13 +959,13 @@
         <v>17</v>
       </c>
       <c r="C13">
-        <v>66</v>
+        <v>34</v>
       </c>
       <c r="D13">
-        <v>48954.92643617148</v>
+        <v>68839.54093644682</v>
       </c>
       <c r="E13" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F13" s="2">
         <v>43842</v>
@@ -979,13 +979,13 @@
         <v>18</v>
       </c>
       <c r="C14">
-        <v>79</v>
+        <v>45</v>
       </c>
       <c r="D14">
-        <v>57394.03987810932</v>
+        <v>42468.91682042312</v>
       </c>
       <c r="E14" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="F14" s="2">
         <v>43843</v>
@@ -999,13 +999,13 @@
         <v>19</v>
       </c>
       <c r="C15">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="D15">
-        <v>66003.30251253414</v>
+        <v>54538.86880278908</v>
       </c>
       <c r="E15" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="F15" s="2">
         <v>43844</v>
@@ -1019,13 +1019,13 @@
         <v>20</v>
       </c>
       <c r="C16">
-        <v>42</v>
+        <v>18</v>
       </c>
       <c r="D16">
-        <v>76106.4908087153</v>
+        <v>28972.8452198771</v>
       </c>
       <c r="E16" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F16" s="2">
         <v>43845</v>
@@ -1039,13 +1039,13 @@
         <v>21</v>
       </c>
       <c r="C17">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="D17">
-        <v>37974.94259573935</v>
+        <v>38294.83680361554</v>
       </c>
       <c r="E17" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F17" s="2">
         <v>43846</v>
@@ -1059,10 +1059,10 @@
         <v>22</v>
       </c>
       <c r="C18">
-        <v>65</v>
+        <v>36</v>
       </c>
       <c r="D18">
-        <v>49727.09320110123</v>
+        <v>71448.34099097823</v>
       </c>
       <c r="E18" t="s">
         <v>107</v>
@@ -1079,13 +1079,13 @@
         <v>23</v>
       </c>
       <c r="C19">
-        <v>70</v>
+        <v>43</v>
       </c>
       <c r="D19">
-        <v>55419.93278191846</v>
+        <v>20049.83749832205</v>
       </c>
       <c r="E19" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F19" s="2">
         <v>43848</v>
@@ -1099,10 +1099,10 @@
         <v>24</v>
       </c>
       <c r="C20">
-        <v>71</v>
+        <v>52</v>
       </c>
       <c r="D20">
-        <v>24820.48877095665</v>
+        <v>73299.51510446113</v>
       </c>
       <c r="E20" t="s">
         <v>109</v>
@@ -1119,10 +1119,10 @@
         <v>25</v>
       </c>
       <c r="C21">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="D21">
-        <v>30483.24086626612</v>
+        <v>74818.80570785355</v>
       </c>
       <c r="E21" t="s">
         <v>107</v>
@@ -1139,13 +1139,13 @@
         <v>26</v>
       </c>
       <c r="C22">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D22">
-        <v>58707.34463788044</v>
+        <v>45101.6998251337</v>
       </c>
       <c r="E22" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="F22" s="2">
         <v>43851</v>
@@ -1159,13 +1159,13 @@
         <v>27</v>
       </c>
       <c r="C23">
-        <v>34</v>
+        <v>63</v>
       </c>
       <c r="D23">
-        <v>45877.08242511524</v>
+        <v>32951.84158123507</v>
       </c>
       <c r="E23" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F23" s="2">
         <v>43852</v>
@@ -1179,13 +1179,13 @@
         <v>28</v>
       </c>
       <c r="C24">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="D24">
-        <v>54612.82791809054</v>
+        <v>64885.29865726946</v>
       </c>
       <c r="E24" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F24" s="2">
         <v>43853</v>
@@ -1199,13 +1199,13 @@
         <v>29</v>
       </c>
       <c r="C25">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="D25">
-        <v>50536.93240885506</v>
+        <v>73866.91554716376</v>
       </c>
       <c r="E25" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F25" s="2">
         <v>43854</v>
@@ -1219,13 +1219,13 @@
         <v>30</v>
       </c>
       <c r="C26">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="D26">
-        <v>40205.76151300374</v>
+        <v>42197.88145378101</v>
       </c>
       <c r="E26" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F26" s="2">
         <v>43855</v>
@@ -1239,13 +1239,13 @@
         <v>31</v>
       </c>
       <c r="C27">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="D27">
-        <v>45683.19115179289</v>
+        <v>37395.76053328079</v>
       </c>
       <c r="E27" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="F27" s="2">
         <v>43856</v>
@@ -1259,13 +1259,13 @@
         <v>32</v>
       </c>
       <c r="C28">
-        <v>49</v>
+        <v>28</v>
       </c>
       <c r="D28">
-        <v>58657.90180678253</v>
+        <v>49962.0555031494</v>
       </c>
       <c r="E28" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F28" s="2">
         <v>43857</v>
@@ -1279,13 +1279,13 @@
         <v>33</v>
       </c>
       <c r="C29">
-        <v>30</v>
+        <v>77</v>
       </c>
       <c r="D29">
-        <v>48271.56622727837</v>
+        <v>85802.37958569446</v>
       </c>
       <c r="E29" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="F29" s="2">
         <v>43858</v>
@@ -1299,10 +1299,10 @@
         <v>34</v>
       </c>
       <c r="C30">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D30">
-        <v>74701.72870016415</v>
+        <v>47071.13735285925</v>
       </c>
       <c r="E30" t="s">
         <v>109</v>
@@ -1319,10 +1319,10 @@
         <v>35</v>
       </c>
       <c r="C31">
-        <v>60</v>
+        <v>34</v>
       </c>
       <c r="D31">
-        <v>52248.92793883236</v>
+        <v>55751.38012955315</v>
       </c>
       <c r="E31" t="s">
         <v>107</v>
@@ -1339,13 +1339,13 @@
         <v>36</v>
       </c>
       <c r="C32">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D32">
-        <v>44076.65232740857</v>
+        <v>46796.09480316775</v>
       </c>
       <c r="E32" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F32" s="2">
         <v>43861</v>
@@ -1359,13 +1359,13 @@
         <v>37</v>
       </c>
       <c r="C33">
-        <v>69</v>
+        <v>41</v>
       </c>
       <c r="D33">
-        <v>48351.04267652005</v>
+        <v>45106.39734880111</v>
       </c>
       <c r="E33" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F33" s="2">
         <v>43862</v>
@@ -1379,13 +1379,13 @@
         <v>38</v>
       </c>
       <c r="C34">
-        <v>27</v>
+        <v>72</v>
       </c>
       <c r="D34">
-        <v>75453.79162114496</v>
+        <v>49052.88947064713</v>
       </c>
       <c r="E34" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F34" s="2">
         <v>43863</v>
@@ -1399,13 +1399,13 @@
         <v>39</v>
       </c>
       <c r="C35">
-        <v>31</v>
+        <v>55</v>
       </c>
       <c r="D35">
-        <v>51868.51563447832</v>
+        <v>18671.86507076199</v>
       </c>
       <c r="E35" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="F35" s="2">
         <v>43864</v>
@@ -1419,10 +1419,10 @@
         <v>40</v>
       </c>
       <c r="C36">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D36">
-        <v>44240.35769429223</v>
+        <v>58030.56434660076</v>
       </c>
       <c r="E36" t="s">
         <v>108</v>
@@ -1442,10 +1442,10 @@
         <v>51</v>
       </c>
       <c r="D37">
-        <v>44068.0230035108</v>
+        <v>68548.41494286804</v>
       </c>
       <c r="E37" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F37" s="2">
         <v>43866</v>
@@ -1459,13 +1459,13 @@
         <v>42</v>
       </c>
       <c r="C38">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D38">
-        <v>26106.2948788011</v>
+        <v>52847.70261492647</v>
       </c>
       <c r="E38" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F38" s="2">
         <v>43867</v>
@@ -1479,13 +1479,13 @@
         <v>43</v>
       </c>
       <c r="C39">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="D39">
-        <v>42338.54729184557</v>
+        <v>73984.24166009335</v>
       </c>
       <c r="E39" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F39" s="2">
         <v>43868</v>
@@ -1499,13 +1499,13 @@
         <v>44</v>
       </c>
       <c r="C40">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="D40">
-        <v>42100.47501351068</v>
+        <v>36611.78510351772</v>
       </c>
       <c r="E40" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F40" s="2">
         <v>43869</v>
@@ -1519,10 +1519,10 @@
         <v>45</v>
       </c>
       <c r="C41">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D41">
-        <v>37488.68423274305</v>
+        <v>32347.32886421066</v>
       </c>
       <c r="E41" t="s">
         <v>108</v>
@@ -1539,13 +1539,13 @@
         <v>46</v>
       </c>
       <c r="C42">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="D42">
-        <v>44692.32837721633</v>
+        <v>16014.71289464421</v>
       </c>
       <c r="E42" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="F42" s="2">
         <v>43871</v>
@@ -1559,10 +1559,10 @@
         <v>47</v>
       </c>
       <c r="C43">
-        <v>58</v>
+        <v>76</v>
       </c>
       <c r="D43">
-        <v>64432.32209770061</v>
+        <v>50609.58473734656</v>
       </c>
       <c r="E43" t="s">
         <v>109</v>
@@ -1579,13 +1579,13 @@
         <v>48</v>
       </c>
       <c r="C44">
-        <v>33</v>
+        <v>67</v>
       </c>
       <c r="D44">
-        <v>43703.51560224265</v>
+        <v>25241.83157721944</v>
       </c>
       <c r="E44" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F44" s="2">
         <v>43873</v>
@@ -1599,13 +1599,13 @@
         <v>49</v>
       </c>
       <c r="C45">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="D45">
-        <v>66303.8898756206</v>
+        <v>60977.9947662164</v>
       </c>
       <c r="E45" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F45" s="2">
         <v>43874</v>
@@ -1619,13 +1619,13 @@
         <v>50</v>
       </c>
       <c r="C46">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="D46">
-        <v>46923.57744112596</v>
+        <v>23120.94502532357</v>
       </c>
       <c r="E46" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F46" s="2">
         <v>43875</v>
@@ -1639,13 +1639,13 @@
         <v>51</v>
       </c>
       <c r="C47">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="D47">
-        <v>43995.35986734502</v>
+        <v>42630.18346802489</v>
       </c>
       <c r="E47" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="F47" s="2">
         <v>43876</v>
@@ -1659,10 +1659,10 @@
         <v>52</v>
       </c>
       <c r="C48">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D48">
-        <v>55270.7790206893</v>
+        <v>48390.69536581478</v>
       </c>
       <c r="E48" t="s">
         <v>107</v>
@@ -1679,13 +1679,13 @@
         <v>53</v>
       </c>
       <c r="C49">
-        <v>20</v>
+        <v>49</v>
       </c>
       <c r="D49">
-        <v>53407.35998381794</v>
+        <v>50716.68038014461</v>
       </c>
       <c r="E49" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="F49" s="2">
         <v>43878</v>
@@ -1699,10 +1699,10 @@
         <v>54</v>
       </c>
       <c r="C50">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="D50">
-        <v>58649.62905401859</v>
+        <v>47088.64253828743</v>
       </c>
       <c r="E50" t="s">
         <v>109</v>
@@ -1719,13 +1719,13 @@
         <v>55</v>
       </c>
       <c r="C51">
-        <v>79</v>
+        <v>42</v>
       </c>
       <c r="D51">
-        <v>47292.78526195467</v>
+        <v>70600.65485066987</v>
       </c>
       <c r="E51" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F51" s="2">
         <v>43880</v>
@@ -1739,13 +1739,13 @@
         <v>56</v>
       </c>
       <c r="C52">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="D52">
-        <v>66402.01494979244</v>
+        <v>73940.14472117049</v>
       </c>
       <c r="E52" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="F52" s="2">
         <v>43881</v>
@@ -1759,13 +1759,13 @@
         <v>57</v>
       </c>
       <c r="C53">
-        <v>26</v>
+        <v>65</v>
       </c>
       <c r="D53">
-        <v>58592.40649883598</v>
+        <v>36115.56379376598</v>
       </c>
       <c r="E53" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="F53" s="2">
         <v>43882</v>
@@ -1779,13 +1779,13 @@
         <v>58</v>
       </c>
       <c r="C54">
-        <v>69</v>
+        <v>20</v>
       </c>
       <c r="D54">
-        <v>17370.19045502302</v>
+        <v>51800.6160850275</v>
       </c>
       <c r="E54" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F54" s="2">
         <v>43883</v>
@@ -1799,13 +1799,13 @@
         <v>59</v>
       </c>
       <c r="C55">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D55">
-        <v>55735.52955027772</v>
+        <v>64642.79572001297</v>
       </c>
       <c r="E55" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F55" s="2">
         <v>43884</v>
@@ -1819,13 +1819,13 @@
         <v>60</v>
       </c>
       <c r="C56">
-        <v>59</v>
+        <v>20</v>
       </c>
       <c r="D56">
-        <v>75591.10503927633</v>
+        <v>43606.24365258857</v>
       </c>
       <c r="E56" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F56" s="2">
         <v>43885</v>
@@ -1839,13 +1839,13 @@
         <v>61</v>
       </c>
       <c r="C57">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="D57">
-        <v>23218.3841255811</v>
+        <v>72566.12708952522</v>
       </c>
       <c r="E57" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F57" s="2">
         <v>43886</v>
@@ -1859,13 +1859,13 @@
         <v>62</v>
       </c>
       <c r="C58">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="D58">
-        <v>48588.11477565604</v>
+        <v>57148.41362827638</v>
       </c>
       <c r="E58" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F58" s="2">
         <v>43887</v>
@@ -1879,13 +1879,13 @@
         <v>63</v>
       </c>
       <c r="C59">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="D59">
-        <v>68325.24692597923</v>
+        <v>41627.24405618266</v>
       </c>
       <c r="E59" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F59" s="2">
         <v>43888</v>
@@ -1899,13 +1899,13 @@
         <v>64</v>
       </c>
       <c r="C60">
-        <v>31</v>
+        <v>71</v>
       </c>
       <c r="D60">
-        <v>30365.90308041511</v>
+        <v>71676.01402008759</v>
       </c>
       <c r="E60" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F60" s="2">
         <v>43889</v>
@@ -1919,13 +1919,13 @@
         <v>65</v>
       </c>
       <c r="C61">
-        <v>42</v>
+        <v>75</v>
       </c>
       <c r="D61">
-        <v>53450.3740104595</v>
+        <v>31753.65030786011</v>
       </c>
       <c r="E61" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="F61" s="2">
         <v>43890</v>
@@ -1939,13 +1939,13 @@
         <v>66</v>
       </c>
       <c r="C62">
-        <v>71</v>
+        <v>50</v>
       </c>
       <c r="D62">
-        <v>51346.86825332633</v>
+        <v>57495.65817626926</v>
       </c>
       <c r="E62" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F62" s="2">
         <v>43891</v>
@@ -1959,13 +1959,13 @@
         <v>67</v>
       </c>
       <c r="C63">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D63">
-        <v>27810.24870253533</v>
+        <v>47158.03711135467</v>
       </c>
       <c r="E63" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F63" s="2">
         <v>43892</v>
@@ -1979,13 +1979,13 @@
         <v>68</v>
       </c>
       <c r="C64">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="D64">
-        <v>52272.05102981208</v>
+        <v>73758.03649826859</v>
       </c>
       <c r="E64" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="F64" s="2">
         <v>43893</v>
@@ -1999,13 +1999,13 @@
         <v>69</v>
       </c>
       <c r="C65">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="D65">
-        <v>41657.98993676054</v>
+        <v>56195.47538872393</v>
       </c>
       <c r="E65" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F65" s="2">
         <v>43894</v>
@@ -2019,10 +2019,10 @@
         <v>70</v>
       </c>
       <c r="C66">
-        <v>77</v>
+        <v>30</v>
       </c>
       <c r="D66">
-        <v>51057.19352143582</v>
+        <v>56244.63154915949</v>
       </c>
       <c r="E66" t="s">
         <v>109</v>
@@ -2039,13 +2039,13 @@
         <v>71</v>
       </c>
       <c r="C67">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="D67">
-        <v>59012.86238532885</v>
+        <v>66542.8759264438</v>
       </c>
       <c r="E67" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F67" s="2">
         <v>43896</v>
@@ -2059,13 +2059,13 @@
         <v>72</v>
       </c>
       <c r="C68">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="D68">
-        <v>40365.29060390065</v>
+        <v>29061.66266984992</v>
       </c>
       <c r="E68" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="F68" s="2">
         <v>43897</v>
@@ -2079,13 +2079,13 @@
         <v>73</v>
       </c>
       <c r="C69">
-        <v>27</v>
+        <v>63</v>
       </c>
       <c r="D69">
-        <v>70471.34954850469</v>
+        <v>25655.47033616016</v>
       </c>
       <c r="E69" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="F69" s="2">
         <v>43898</v>
@@ -2099,13 +2099,13 @@
         <v>74</v>
       </c>
       <c r="C70">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="D70">
-        <v>63240.0812537862</v>
+        <v>68506.16078819877</v>
       </c>
       <c r="E70" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F70" s="2">
         <v>43899</v>
@@ -2122,10 +2122,10 @@
         <v>72</v>
       </c>
       <c r="D71">
-        <v>18179.35467187743</v>
+        <v>71994.73507488299</v>
       </c>
       <c r="E71" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="F71" s="2">
         <v>43900</v>
@@ -2139,13 +2139,13 @@
         <v>76</v>
       </c>
       <c r="C72">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="D72">
-        <v>32283.42795166735</v>
+        <v>20836.27538595467</v>
       </c>
       <c r="E72" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="F72" s="2">
         <v>43901</v>
@@ -2159,10 +2159,10 @@
         <v>77</v>
       </c>
       <c r="C73">
-        <v>40</v>
+        <v>66</v>
       </c>
       <c r="D73">
-        <v>48505.75160779511</v>
+        <v>23761.17854227098</v>
       </c>
       <c r="E73" t="s">
         <v>107</v>
@@ -2179,13 +2179,13 @@
         <v>78</v>
       </c>
       <c r="C74">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="D74">
-        <v>44246.66518414129</v>
+        <v>47519.68310784522</v>
       </c>
       <c r="E74" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="F74" s="2">
         <v>43903</v>
@@ -2199,13 +2199,13 @@
         <v>79</v>
       </c>
       <c r="C75">
-        <v>75</v>
+        <v>40</v>
       </c>
       <c r="D75">
-        <v>69432.78611348041</v>
+        <v>33751.34822343578</v>
       </c>
       <c r="E75" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F75" s="2">
         <v>43904</v>
@@ -2219,13 +2219,13 @@
         <v>80</v>
       </c>
       <c r="C76">
-        <v>24</v>
+        <v>49</v>
       </c>
       <c r="D76">
-        <v>30304.04661424935</v>
+        <v>101688.8720677126</v>
       </c>
       <c r="E76" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="F76" s="2">
         <v>43905</v>
@@ -2239,13 +2239,13 @@
         <v>81</v>
       </c>
       <c r="C77">
-        <v>79</v>
+        <v>57</v>
       </c>
       <c r="D77">
-        <v>73564.44534065215</v>
+        <v>50999.06825888675</v>
       </c>
       <c r="E77" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F77" s="2">
         <v>43906</v>
@@ -2259,10 +2259,10 @@
         <v>82</v>
       </c>
       <c r="C78">
-        <v>24</v>
+        <v>65</v>
       </c>
       <c r="D78">
-        <v>49191.81854892011</v>
+        <v>64440.66470838438</v>
       </c>
       <c r="E78" t="s">
         <v>108</v>
@@ -2279,10 +2279,10 @@
         <v>83</v>
       </c>
       <c r="C79">
-        <v>71</v>
+        <v>18</v>
       </c>
       <c r="D79">
-        <v>50661.34144889322</v>
+        <v>77729.8496574509</v>
       </c>
       <c r="E79" t="s">
         <v>107</v>
@@ -2299,10 +2299,10 @@
         <v>84</v>
       </c>
       <c r="C80">
-        <v>74</v>
+        <v>35</v>
       </c>
       <c r="D80">
-        <v>48673.44467474732</v>
+        <v>49770.01158891532</v>
       </c>
       <c r="E80" t="s">
         <v>108</v>
@@ -2319,13 +2319,13 @@
         <v>85</v>
       </c>
       <c r="C81">
-        <v>54</v>
+        <v>74</v>
       </c>
       <c r="D81">
-        <v>98963.20347428897</v>
+        <v>81052.83567745384</v>
       </c>
       <c r="E81" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F81" s="2">
         <v>43910</v>
@@ -2339,13 +2339,13 @@
         <v>86</v>
       </c>
       <c r="C82">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="D82">
-        <v>55679.36071724434</v>
+        <v>34868.69025124405</v>
       </c>
       <c r="E82" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F82" s="2">
         <v>43911</v>
@@ -2359,10 +2359,10 @@
         <v>87</v>
       </c>
       <c r="C83">
-        <v>30</v>
+        <v>74</v>
       </c>
       <c r="D83">
-        <v>67779.97485371451</v>
+        <v>35377.0717491775</v>
       </c>
       <c r="E83" t="s">
         <v>106</v>
@@ -2379,10 +2379,10 @@
         <v>88</v>
       </c>
       <c r="C84">
-        <v>24</v>
+        <v>55</v>
       </c>
       <c r="D84">
-        <v>32124.29550752011</v>
+        <v>23507.09893297654</v>
       </c>
       <c r="E84" t="s">
         <v>106</v>
@@ -2399,13 +2399,13 @@
         <v>89</v>
       </c>
       <c r="C85">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D85">
-        <v>29127.37378302239</v>
+        <v>59890.6056571598</v>
       </c>
       <c r="E85" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F85" s="2">
         <v>43914</v>
@@ -2419,13 +2419,13 @@
         <v>90</v>
       </c>
       <c r="C86">
-        <v>55</v>
+        <v>27</v>
       </c>
       <c r="D86">
-        <v>63869.86919970914</v>
+        <v>43509.46385885791</v>
       </c>
       <c r="E86" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="F86" s="2">
         <v>43915</v>
@@ -2439,10 +2439,10 @@
         <v>91</v>
       </c>
       <c r="C87">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="D87">
-        <v>65305.27815109371</v>
+        <v>44532.09385749022</v>
       </c>
       <c r="E87" t="s">
         <v>109</v>
@@ -2459,10 +2459,10 @@
         <v>92</v>
       </c>
       <c r="C88">
-        <v>22</v>
+        <v>49</v>
       </c>
       <c r="D88">
-        <v>60117.76379040501</v>
+        <v>54992.8557169707</v>
       </c>
       <c r="E88" t="s">
         <v>109</v>
@@ -2479,10 +2479,10 @@
         <v>93</v>
       </c>
       <c r="C89">
-        <v>52</v>
+        <v>74</v>
       </c>
       <c r="D89">
-        <v>70767.2903418934</v>
+        <v>26930.25873930648</v>
       </c>
       <c r="E89" t="s">
         <v>108</v>
@@ -2499,13 +2499,13 @@
         <v>94</v>
       </c>
       <c r="C90">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D90">
-        <v>56077.91040792828</v>
+        <v>45892.37162788925</v>
       </c>
       <c r="E90" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F90" s="2">
         <v>43919</v>
@@ -2519,13 +2519,13 @@
         <v>95</v>
       </c>
       <c r="C91">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D91">
-        <v>67006.05251907</v>
+        <v>57658.35543176521</v>
       </c>
       <c r="E91" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F91" s="2">
         <v>43920</v>
@@ -2539,13 +2539,13 @@
         <v>96</v>
       </c>
       <c r="C92">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D92">
-        <v>49432.64048422922</v>
+        <v>29817.29369056463</v>
       </c>
       <c r="E92" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="F92" s="2">
         <v>43921</v>
@@ -2559,13 +2559,13 @@
         <v>97</v>
       </c>
       <c r="C93">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="D93">
-        <v>66136.33221684038</v>
+        <v>25280.47072357372</v>
       </c>
       <c r="E93" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F93" s="2">
         <v>43922</v>
@@ -2579,10 +2579,10 @@
         <v>98</v>
       </c>
       <c r="C94">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="D94">
-        <v>32687.47473736109</v>
+        <v>41004.51535889443</v>
       </c>
       <c r="E94" t="s">
         <v>109</v>
@@ -2599,13 +2599,13 @@
         <v>99</v>
       </c>
       <c r="C95">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="D95">
-        <v>52670.5250475358</v>
+        <v>38553.22925857084</v>
       </c>
       <c r="E95" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F95" s="2">
         <v>43924</v>
@@ -2619,13 +2619,13 @@
         <v>100</v>
       </c>
       <c r="C96">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="D96">
-        <v>54613.10580325167</v>
+        <v>43089.37059986212</v>
       </c>
       <c r="E96" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F96" s="2">
         <v>43925</v>
@@ -2639,13 +2639,13 @@
         <v>101</v>
       </c>
       <c r="C97">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="D97">
-        <v>65068.88290094392</v>
+        <v>36162.48166826696</v>
       </c>
       <c r="E97" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="F97" s="2">
         <v>43926</v>
@@ -2659,13 +2659,13 @@
         <v>102</v>
       </c>
       <c r="C98">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D98">
-        <v>34097.00250480168</v>
+        <v>55994.56722742079</v>
       </c>
       <c r="E98" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="F98" s="2">
         <v>43927</v>
@@ -2679,10 +2679,10 @@
         <v>103</v>
       </c>
       <c r="C99">
-        <v>66</v>
+        <v>36</v>
       </c>
       <c r="D99">
-        <v>59088.015848345</v>
+        <v>57250.01650165959</v>
       </c>
       <c r="E99" t="s">
         <v>108</v>
@@ -2699,10 +2699,10 @@
         <v>104</v>
       </c>
       <c r="C100">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="D100">
-        <v>49830.41177271114</v>
+        <v>48500.54077651552</v>
       </c>
       <c r="E100" t="s">
         <v>109</v>
@@ -2719,10 +2719,10 @@
         <v>105</v>
       </c>
       <c r="C101">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="D101">
-        <v>44937.84612627549</v>
+        <v>87885.06584167352</v>
       </c>
       <c r="E101" t="s">
         <v>109</v>

</xml_diff>